<commit_message>
Docstrings for alpha_package_costs.py. Revise alpha_package_costs.py such that input files won't build with autodoc. Revise make_hev_from_alpha_ice.py to work with new input structure withint alpha_package_costs.py. Revise alpha_package_costs_module_inputs.xlsx to remove some unused entries.
</commit_message>
<xml_diff>
--- a/omega_preproc/alpha_package_costs/inputs/alpha_package_costs_module_inputs.xlsx
+++ b/omega_preproc/alpha_package_costs/inputs/alpha_package_costs_module_inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TSHERWOO\PycharmProjects\EPA_OMEGA_Model\omega_preproc\alpha_package_costs\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91027E3E-C5AA-4568-A301-73D811025453}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFBF0AEB-7ABB-48AD-9533-8D91BEDD47F4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="826" firstSheet="1" activeTab="10" xr2:uid="{31AE0ECC-ADD6-46A3-9F50-4BA6582DDF8B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="826" activeTab="5" xr2:uid="{31AE0ECC-ADD6-46A3-9F50-4BA6582DDF8B}"/>
   </bookViews>
   <sheets>
     <sheet name="inputs_code" sheetId="15" r:id="rId1"/>
@@ -38,12 +38,12 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="16" hidden="1">aero!$B$1:$E$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="17" hidden="1">nonaero!$C$1:$E$4</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">trans!$A$1:$H$91</definedName>
-    <definedName name="AWD_scaler">inputs_workbook!$B$6</definedName>
+    <definedName name="AWD_scaler">inputs_workbook!$B$3</definedName>
     <definedName name="Markup">inputs_workbook!$B$1</definedName>
-    <definedName name="Null_4cyl_DMC">inputs_workbook!$B$4</definedName>
-    <definedName name="Null_6cyl_DMC">inputs_workbook!$B$3</definedName>
-    <definedName name="Null_8cyl_DMC">inputs_workbook!$B$2</definedName>
-    <definedName name="TRX10_">inputs_workbook!$B$5</definedName>
+    <definedName name="Null_4cyl_DMC">inputs_workbook!#REF!</definedName>
+    <definedName name="Null_6cyl_DMC">inputs_workbook!#REF!</definedName>
+    <definedName name="Null_8cyl_DMC">inputs_workbook!#REF!</definedName>
+    <definedName name="TRX10_">inputs_workbook!$B$2</definedName>
     <definedName name="workbook_dollar_basis">inputs_workbook!#REF!</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -293,7 +293,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="955" uniqueCount="329">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="948" uniqueCount="322">
   <si>
     <t>Markup</t>
   </si>
@@ -799,15 +799,6 @@
     <t>360_ClassNA</t>
   </si>
   <si>
-    <t>Null_8cyl_DMC</t>
-  </si>
-  <si>
-    <t>Null_6cyl_DMC</t>
-  </si>
-  <si>
-    <t>Null_4cyl_DMC</t>
-  </si>
-  <si>
     <t>dmc</t>
   </si>
   <si>
@@ -1132,9 +1123,6 @@
     <t>dollars_per_kWh_curve</t>
   </si>
   <si>
-    <t>dollars_per_kW_curve</t>
-  </si>
-  <si>
     <t>run_ID</t>
   </si>
   <si>
@@ -1144,9 +1132,6 @@
     <t>usable_soc_bev</t>
   </si>
   <si>
-    <t>charging_loss_bev</t>
-  </si>
-  <si>
     <t>gap_bev</t>
   </si>
   <si>
@@ -1156,9 +1141,6 @@
     <t>usable_soc_hev</t>
   </si>
   <si>
-    <t>charging_loss_hev</t>
-  </si>
-  <si>
     <t>gap_hev</t>
   </si>
   <si>
@@ -1168,9 +1150,6 @@
     <t>usable_soc_phev</t>
   </si>
   <si>
-    <t>charging_loss_phev</t>
-  </si>
-  <si>
     <t>gap_phev</t>
   </si>
   <si>
@@ -1183,103 +1162,103 @@
     <t>co2_reduction_hwy_hev</t>
   </si>
   <si>
+    <t>kWh_pack_per_kg_pack_curve</t>
+  </si>
+  <si>
+    <t>co2_reduction_cycle_hev</t>
+  </si>
+  <si>
+    <t>slope</t>
+  </si>
+  <si>
+    <t>intercept</t>
+  </si>
+  <si>
+    <t>Motor kW</t>
+  </si>
+  <si>
+    <t>DCDC converter kW (3.5)</t>
+  </si>
+  <si>
+    <t>Vehicle size class (1-7)</t>
+  </si>
+  <si>
+    <t>HVAC</t>
+  </si>
+  <si>
+    <t>none at this time</t>
+  </si>
+  <si>
+    <t>quantity</t>
+  </si>
+  <si>
+    <t>scale_by</t>
+  </si>
+  <si>
+    <t>DCDC_converter</t>
+  </si>
+  <si>
+    <t>HV_orange_cables</t>
+  </si>
+  <si>
+    <t>LV_battery</t>
+  </si>
+  <si>
+    <t>kW_DCDC_converter</t>
+  </si>
+  <si>
+    <t>motor</t>
+  </si>
+  <si>
+    <t>inverter</t>
+  </si>
+  <si>
+    <t>induction_motor</t>
+  </si>
+  <si>
+    <t>induction_inverter</t>
+  </si>
+  <si>
+    <t>single_speed_gearbox</t>
+  </si>
+  <si>
+    <t>powertrain_cooling_loop</t>
+  </si>
+  <si>
+    <t>DC_fast_charge_circuitry</t>
+  </si>
+  <si>
+    <t>power_management_and_distribution</t>
+  </si>
+  <si>
+    <t>additional_pair_of_half_shafts</t>
+  </si>
+  <si>
+    <t>brake_sensors_actuators</t>
+  </si>
+  <si>
+    <t>charging_cord_kit</t>
+  </si>
+  <si>
+    <t>Vehicle kW</t>
+  </si>
+  <si>
+    <t>DC-DC kW (3.5) + OBC kW (7,11,19)</t>
+  </si>
+  <si>
+    <t>Vehicle kW / 2</t>
+  </si>
+  <si>
+    <t>DeacFC</t>
+  </si>
+  <si>
+    <t>AddingDeacFC</t>
+  </si>
+  <si>
     <t>kWh_pack_per_kg_curbwt_curve</t>
   </si>
   <si>
     <t>kW_motor_per_kg_curbwt_curve</t>
-  </si>
-  <si>
-    <t>kWh_pack_per_kg_pack_curve</t>
-  </si>
-  <si>
-    <t>co2_reduction_cycle_hev</t>
-  </si>
-  <si>
-    <t>slope</t>
-  </si>
-  <si>
-    <t>intercept</t>
-  </si>
-  <si>
-    <t>Motor kW</t>
-  </si>
-  <si>
-    <t>DCDC converter kW (3.5)</t>
-  </si>
-  <si>
-    <t>Vehicle size class (1-7)</t>
-  </si>
-  <si>
-    <t>HVAC</t>
-  </si>
-  <si>
-    <t>none at this time</t>
-  </si>
-  <si>
-    <t>quantity</t>
-  </si>
-  <si>
-    <t>scale_by</t>
-  </si>
-  <si>
-    <t>DCDC_converter</t>
-  </si>
-  <si>
-    <t>HV_orange_cables</t>
-  </si>
-  <si>
-    <t>LV_battery</t>
-  </si>
-  <si>
-    <t>kW_DCDC_converter</t>
-  </si>
-  <si>
-    <t>motor</t>
-  </si>
-  <si>
-    <t>inverter</t>
-  </si>
-  <si>
-    <t>induction_motor</t>
-  </si>
-  <si>
-    <t>induction_inverter</t>
-  </si>
-  <si>
-    <t>single_speed_gearbox</t>
-  </si>
-  <si>
-    <t>powertrain_cooling_loop</t>
-  </si>
-  <si>
-    <t>DC_fast_charge_circuitry</t>
-  </si>
-  <si>
-    <t>power_management_and_distribution</t>
-  </si>
-  <si>
-    <t>additional_pair_of_half_shafts</t>
-  </si>
-  <si>
-    <t>brake_sensors_actuators</t>
-  </si>
-  <si>
-    <t>charging_cord_kit</t>
-  </si>
-  <si>
-    <t>Vehicle kW</t>
-  </si>
-  <si>
-    <t>DC-DC kW (3.5) + OBC kW (7,11,19)</t>
-  </si>
-  <si>
-    <t>Vehicle kW / 2</t>
-  </si>
-  <si>
-    <t>DeacFC</t>
-  </si>
-  <si>
-    <t>AddingDeacFC</t>
   </si>
 </sst>
 </file>
@@ -1947,7 +1926,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A2" sqref="A2:A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1957,29 +1936,29 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="B1" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>328</v>
+        <v>319</v>
       </c>
     </row>
     <row r="3" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="B3" s="1"/>
     </row>
     <row r="4" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="B4" s="1">
         <v>2020</v>
@@ -1987,7 +1966,7 @@
     </row>
     <row r="5" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="B5" s="1">
         <v>2050</v>
@@ -1995,7 +1974,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="B6" s="1">
         <v>5.0000000000000001E-3</v>
@@ -2003,7 +1982,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="B7" s="1">
         <v>0.01</v>
@@ -2011,7 +1990,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="B8" s="1">
         <v>1.4999999999999999E-2</v>
@@ -2019,7 +1998,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="B9" s="1">
         <v>2.5000000000000001E-2</v>
@@ -2027,7 +2006,7 @@
     </row>
     <row r="10" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="B10" s="1">
         <v>1.2</v>
@@ -2035,7 +2014,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2044,17 +2024,17 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="B1" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -2062,7 +2042,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0.8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -2078,7 +2058,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -2086,7 +2066,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -2098,7 +2078,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{790C9274-B2D0-4CB1-A413-BFF03ACE11B8}">
   <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
@@ -2111,21 +2091,21 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="B2" s="4">
         <f t="shared" ref="B2:B23" si="0">Markup*C2</f>
@@ -2140,7 +2120,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="B3" s="4">
         <f t="shared" si="0"/>
@@ -2155,7 +2135,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="B4" s="4">
         <f t="shared" si="0"/>
@@ -2170,7 +2150,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="B5" s="4">
         <f t="shared" si="0"/>
@@ -2185,7 +2165,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="B6" s="4">
         <f t="shared" si="0"/>
@@ -2200,7 +2180,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="B7" s="7">
         <f t="shared" si="0"/>
@@ -2215,7 +2195,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="B8" s="7">
         <f t="shared" si="0"/>
@@ -2230,7 +2210,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="B9" s="7">
         <f t="shared" si="0"/>
@@ -2245,7 +2225,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="B10" s="7">
         <f t="shared" si="0"/>
@@ -2260,7 +2240,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="B11" s="7">
         <f t="shared" si="0"/>
@@ -2275,7 +2255,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="B12" s="7">
         <f t="shared" si="0"/>
@@ -2290,7 +2270,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="10" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="B13" s="7">
         <f t="shared" si="0"/>
@@ -2305,7 +2285,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="10" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="B14" s="7">
         <f t="shared" si="0"/>
@@ -2320,7 +2300,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="B15" s="7">
         <f t="shared" si="0"/>
@@ -2335,7 +2315,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="10" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="B16" s="7">
         <f t="shared" si="0"/>
@@ -2350,7 +2330,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="B17" s="7">
         <f t="shared" si="0"/>
@@ -2365,7 +2345,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="10" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="B18" s="7">
         <f t="shared" si="0"/>
@@ -2380,7 +2360,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="9" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="B19" s="7">
         <f t="shared" si="0"/>
@@ -2395,7 +2375,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="10" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="B20" s="7">
         <f t="shared" si="0"/>
@@ -2410,7 +2390,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="10" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="B21" s="7">
         <f t="shared" si="0"/>
@@ -2425,7 +2405,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="B22" s="7">
         <f t="shared" si="0"/>
@@ -2440,7 +2420,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="10" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B23" s="7">
         <f t="shared" si="0"/>
@@ -2455,7 +2435,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="9" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="B24" s="7">
         <f t="shared" ref="B24:B32" si="1">Markup*C24</f>
@@ -2471,7 +2451,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="9" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="B25" s="7">
         <f t="shared" si="1"/>
@@ -2487,7 +2467,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="9" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="B26" s="7">
         <f t="shared" si="1"/>
@@ -2503,7 +2483,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="9" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="B27" s="7">
         <f t="shared" si="1"/>
@@ -2518,7 +2498,7 @@
     </row>
     <row r="28" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="15" t="s">
-        <v>327</v>
+        <v>318</v>
       </c>
       <c r="B28" s="7">
         <f t="shared" si="1"/>
@@ -2533,7 +2513,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="9" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="B29" s="7">
         <f t="shared" si="1"/>
@@ -2548,7 +2528,7 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="9" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="B30" s="7">
         <f t="shared" si="1"/>
@@ -2563,7 +2543,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="9" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B31" s="7">
         <f t="shared" si="1"/>
@@ -2578,7 +2558,7 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="9" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="B32" s="7">
         <f t="shared" si="1"/>
@@ -2601,7 +2581,7 @@
   <dimension ref="A1:H91"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F90"/>
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2614,28 +2594,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="B1" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="E1" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="F1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -2647,10 +2627,10 @@
         <v>3</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="E2" s="7">
         <f t="shared" ref="E2:E33" si="0">Markup*F2</f>
@@ -2675,10 +2655,10 @@
         <v>3</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="E3" s="7">
         <f t="shared" si="0"/>
@@ -2703,10 +2683,10 @@
         <v>3</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="E4" s="7">
         <f t="shared" si="0"/>
@@ -2731,10 +2711,10 @@
         <v>3</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="E5" s="7">
         <f t="shared" si="0"/>
@@ -2759,10 +2739,10 @@
         <v>3</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E6" s="7">
         <f t="shared" si="0"/>
@@ -2787,10 +2767,10 @@
         <v>3</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="E7" s="7">
         <f t="shared" si="0"/>
@@ -2812,13 +2792,13 @@
         <v>TRX11_FWD_LPW_LRL</v>
       </c>
       <c r="B8" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="E8" s="7">
         <f t="shared" si="0"/>
@@ -2841,13 +2821,13 @@
         <v>TRX11_FWD_LPW_HRL</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="E9" s="7">
         <f t="shared" si="0"/>
@@ -2870,13 +2850,13 @@
         <v>TRX11_FWD_MPW_LRL</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="E10" s="7">
         <f t="shared" si="0"/>
@@ -2899,13 +2879,13 @@
         <v>TRX11_FWD_MPW_HRL</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="E11" s="7">
         <f t="shared" si="0"/>
@@ -2928,13 +2908,13 @@
         <v>TRX11_FWD_HPW</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E12" s="7">
         <f t="shared" si="0"/>
@@ -2957,13 +2937,13 @@
         <v>TRX11_FWD_Truck</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="E13" s="7">
         <f t="shared" si="0"/>
@@ -2986,13 +2966,13 @@
         <v>TRX12_FWD_LPW_LRL</v>
       </c>
       <c r="B14" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="E14" s="7">
         <f t="shared" si="0"/>
@@ -3015,13 +2995,13 @@
         <v>TRX12_FWD_LPW_HRL</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="E15" s="7">
         <f t="shared" si="0"/>
@@ -3044,13 +3024,13 @@
         <v>TRX12_FWD_MPW_LRL</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="E16" s="7">
         <f t="shared" si="0"/>
@@ -3073,13 +3053,13 @@
         <v>TRX12_FWD_MPW_HRL</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="E17" s="7">
         <f t="shared" si="0"/>
@@ -3102,13 +3082,13 @@
         <v>TRX12_FWD_HPW</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E18" s="7">
         <f t="shared" si="0"/>
@@ -3131,13 +3111,13 @@
         <v>TRX12_FWD_Truck</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="E19" s="7">
         <f t="shared" si="0"/>
@@ -3160,13 +3140,13 @@
         <v>TRX21_FWD_LPW_LRL</v>
       </c>
       <c r="B20" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="E20" s="7">
         <f t="shared" si="0"/>
@@ -3189,13 +3169,13 @@
         <v>TRX21_FWD_LPW_HRL</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="E21" s="7">
         <f t="shared" si="0"/>
@@ -3218,13 +3198,13 @@
         <v>TRX21_FWD_MPW_LRL</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="E22" s="7">
         <f t="shared" si="0"/>
@@ -3247,13 +3227,13 @@
         <v>TRX21_FWD_MPW_HRL</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="E23" s="7">
         <f t="shared" si="0"/>
@@ -3276,13 +3256,13 @@
         <v>TRX21_FWD_HPW</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E24" s="7">
         <f t="shared" si="0"/>
@@ -3305,13 +3285,13 @@
         <v>TRX21_FWD_Truck</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="D25" s="10" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="E25" s="7">
         <f t="shared" si="0"/>
@@ -3334,13 +3314,13 @@
         <v>TRX22_FWD_LPW_LRL</v>
       </c>
       <c r="B26" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="E26" s="7">
         <f t="shared" si="0"/>
@@ -3363,13 +3343,13 @@
         <v>TRX22_FWD_LPW_HRL</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="E27" s="7">
         <f t="shared" si="0"/>
@@ -3392,13 +3372,13 @@
         <v>TRX22_FWD_MPW_LRL</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="D28" s="10" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="E28" s="7">
         <f t="shared" si="0"/>
@@ -3421,13 +3401,13 @@
         <v>TRX22_FWD_MPW_HRL</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="D29" s="10" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="E29" s="7">
         <f t="shared" si="0"/>
@@ -3450,13 +3430,13 @@
         <v>TRX22_FWD_HPW</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="D30" s="10" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E30" s="7">
         <f t="shared" si="0"/>
@@ -3479,13 +3459,13 @@
         <v>TRX22_FWD_Truck</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="D31" s="10" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="E31" s="7">
         <f t="shared" si="0"/>
@@ -3511,10 +3491,10 @@
         <v>3</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="D32" s="9" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="E32" s="7">
         <f t="shared" si="0"/>
@@ -3540,10 +3520,10 @@
         <v>3</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="D33" s="9" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="E33" s="7">
         <f t="shared" si="0"/>
@@ -3569,10 +3549,10 @@
         <v>3</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="D34" s="10" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="E34" s="7">
         <f t="shared" ref="E34:E65" si="5">Markup*F34</f>
@@ -3598,10 +3578,10 @@
         <v>3</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="D35" s="10" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="E35" s="7">
         <f t="shared" si="5"/>
@@ -3627,10 +3607,10 @@
         <v>3</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="D36" s="10" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E36" s="7">
         <f t="shared" si="5"/>
@@ -3656,10 +3636,10 @@
         <v>3</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="D37" s="10" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="E37" s="7">
         <f t="shared" si="5"/>
@@ -3682,13 +3662,13 @@
         <v>TRX11_AWD_LPW_LRL</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="D38" s="9" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="E38" s="7">
         <f t="shared" si="5"/>
@@ -3711,13 +3691,13 @@
         <v>TRX11_AWD_LPW_HRL</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="D39" s="9" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="E39" s="7">
         <f t="shared" si="5"/>
@@ -3740,13 +3720,13 @@
         <v>TRX11_AWD_MPW_LRL</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="D40" s="10" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="E40" s="7">
         <f t="shared" si="5"/>
@@ -3769,13 +3749,13 @@
         <v>TRX11_AWD_MPW_HRL</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="D41" s="10" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="E41" s="7">
         <f t="shared" si="5"/>
@@ -3798,13 +3778,13 @@
         <v>TRX11_AWD_HPW</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="D42" s="10" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E42" s="7">
         <f t="shared" si="5"/>
@@ -3827,13 +3807,13 @@
         <v>TRX11_AWD_Truck</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="D43" s="10" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="E43" s="7">
         <f t="shared" si="5"/>
@@ -3856,13 +3836,13 @@
         <v>TRX12_AWD_LPW_LRL</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="C44" s="9" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="D44" s="9" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="E44" s="7">
         <f t="shared" si="5"/>
@@ -3885,13 +3865,13 @@
         <v>TRX12_AWD_LPW_HRL</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="D45" s="9" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="E45" s="7">
         <f t="shared" si="5"/>
@@ -3914,13 +3894,13 @@
         <v>TRX12_AWD_MPW_LRL</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="D46" s="10" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="E46" s="7">
         <f t="shared" si="5"/>
@@ -3943,13 +3923,13 @@
         <v>TRX12_AWD_MPW_HRL</v>
       </c>
       <c r="B47" s="9" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="D47" s="10" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="E47" s="7">
         <f t="shared" si="5"/>
@@ -3972,13 +3952,13 @@
         <v>TRX12_AWD_HPW</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="C48" s="9" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="D48" s="10" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E48" s="7">
         <f t="shared" si="5"/>
@@ -4001,13 +3981,13 @@
         <v>TRX12_AWD_Truck</v>
       </c>
       <c r="B49" s="9" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="C49" s="9" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="D49" s="10" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="E49" s="7">
         <f t="shared" si="5"/>
@@ -4030,13 +4010,13 @@
         <v>TRX21_AWD_LPW_LRL</v>
       </c>
       <c r="B50" s="9" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="C50" s="9" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="D50" s="9" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="E50" s="7">
         <f t="shared" si="5"/>
@@ -4059,13 +4039,13 @@
         <v>TRX21_AWD_LPW_HRL</v>
       </c>
       <c r="B51" s="9" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="C51" s="9" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="D51" s="9" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="E51" s="7">
         <f t="shared" si="5"/>
@@ -4088,13 +4068,13 @@
         <v>TRX21_AWD_MPW_LRL</v>
       </c>
       <c r="B52" s="9" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="C52" s="9" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="D52" s="10" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="E52" s="7">
         <f t="shared" si="5"/>
@@ -4117,13 +4097,13 @@
         <v>TRX21_AWD_MPW_HRL</v>
       </c>
       <c r="B53" s="9" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="D53" s="10" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="E53" s="7">
         <f t="shared" si="5"/>
@@ -4146,13 +4126,13 @@
         <v>TRX21_AWD_HPW</v>
       </c>
       <c r="B54" s="9" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="C54" s="9" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="D54" s="10" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E54" s="7">
         <f t="shared" si="5"/>
@@ -4175,13 +4155,13 @@
         <v>TRX21_AWD_Truck</v>
       </c>
       <c r="B55" s="9" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="C55" s="9" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="D55" s="10" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="E55" s="7">
         <f t="shared" si="5"/>
@@ -4204,13 +4184,13 @@
         <v>TRX22_AWD_LPW_LRL</v>
       </c>
       <c r="B56" s="9" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="C56" s="9" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="D56" s="9" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="E56" s="7">
         <f t="shared" si="5"/>
@@ -4233,13 +4213,13 @@
         <v>TRX22_AWD_LPW_HRL</v>
       </c>
       <c r="B57" s="9" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="D57" s="9" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="E57" s="7">
         <f t="shared" si="5"/>
@@ -4262,13 +4242,13 @@
         <v>TRX22_AWD_MPW_LRL</v>
       </c>
       <c r="B58" s="9" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="C58" s="9" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="D58" s="10" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="E58" s="7">
         <f t="shared" si="5"/>
@@ -4291,13 +4271,13 @@
         <v>TRX22_AWD_MPW_HRL</v>
       </c>
       <c r="B59" s="9" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="C59" s="9" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="D59" s="10" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="E59" s="7">
         <f t="shared" si="5"/>
@@ -4320,13 +4300,13 @@
         <v>TRX22_AWD_HPW</v>
       </c>
       <c r="B60" s="9" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="C60" s="9" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="D60" s="10" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E60" s="7">
         <f t="shared" si="5"/>
@@ -4349,13 +4329,13 @@
         <v>TRX22_AWD_Truck</v>
       </c>
       <c r="B61" s="9" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="C61" s="9" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="D61" s="10" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="E61" s="7">
         <f t="shared" si="5"/>
@@ -4381,10 +4361,10 @@
         <v>3</v>
       </c>
       <c r="C62" s="9" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="D62" s="9" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="E62" s="7">
         <f t="shared" si="5"/>
@@ -4410,10 +4390,10 @@
         <v>3</v>
       </c>
       <c r="C63" s="9" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="D63" s="9" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="E63" s="7">
         <f t="shared" si="5"/>
@@ -4439,10 +4419,10 @@
         <v>3</v>
       </c>
       <c r="C64" s="9" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="D64" s="10" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="E64" s="7">
         <f t="shared" si="5"/>
@@ -4468,10 +4448,10 @@
         <v>3</v>
       </c>
       <c r="C65" s="9" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="D65" s="10" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="E65" s="7">
         <f t="shared" si="5"/>
@@ -4497,10 +4477,10 @@
         <v>3</v>
       </c>
       <c r="C66" s="9" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="D66" s="10" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E66" s="7">
         <f t="shared" ref="E66:E91" si="8">Markup*F66</f>
@@ -4526,10 +4506,10 @@
         <v>3</v>
       </c>
       <c r="C67" s="9" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="D67" s="10" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="E67" s="7">
         <f t="shared" si="8"/>
@@ -4552,13 +4532,13 @@
         <v>TRX11_RWD_LPW_LRL</v>
       </c>
       <c r="B68" s="9" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="C68" s="9" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="D68" s="9" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="E68" s="7">
         <f t="shared" si="8"/>
@@ -4581,13 +4561,13 @@
         <v>TRX11_RWD_LPW_HRL</v>
       </c>
       <c r="B69" s="9" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="C69" s="9" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="D69" s="9" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="E69" s="7">
         <f t="shared" si="8"/>
@@ -4610,13 +4590,13 @@
         <v>TRX11_RWD_MPW_LRL</v>
       </c>
       <c r="B70" s="9" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="C70" s="9" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="D70" s="10" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="E70" s="7">
         <f t="shared" si="8"/>
@@ -4639,13 +4619,13 @@
         <v>TRX11_RWD_MPW_HRL</v>
       </c>
       <c r="B71" s="9" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="C71" s="9" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="D71" s="10" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="E71" s="7">
         <f t="shared" si="8"/>
@@ -4668,13 +4648,13 @@
         <v>TRX11_RWD_HPW</v>
       </c>
       <c r="B72" s="9" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="C72" s="9" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="D72" s="10" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E72" s="7">
         <f t="shared" si="8"/>
@@ -4697,13 +4677,13 @@
         <v>TRX11_RWD_Truck</v>
       </c>
       <c r="B73" s="9" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="C73" s="9" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="D73" s="10" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="E73" s="7">
         <f t="shared" si="8"/>
@@ -4726,13 +4706,13 @@
         <v>TRX12_RWD_LPW_LRL</v>
       </c>
       <c r="B74" s="9" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="C74" s="9" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="D74" s="9" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="E74" s="7">
         <f t="shared" si="8"/>
@@ -4755,13 +4735,13 @@
         <v>TRX12_RWD_LPW_HRL</v>
       </c>
       <c r="B75" s="9" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="C75" s="9" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="D75" s="9" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="E75" s="7">
         <f t="shared" si="8"/>
@@ -4784,13 +4764,13 @@
         <v>TRX12_RWD_MPW_LRL</v>
       </c>
       <c r="B76" s="9" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="C76" s="9" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="D76" s="10" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="E76" s="7">
         <f t="shared" si="8"/>
@@ -4813,13 +4793,13 @@
         <v>TRX12_RWD_MPW_HRL</v>
       </c>
       <c r="B77" s="9" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="C77" s="9" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="D77" s="10" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="E77" s="7">
         <f t="shared" si="8"/>
@@ -4842,13 +4822,13 @@
         <v>TRX12_RWD_HPW</v>
       </c>
       <c r="B78" s="9" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="C78" s="9" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="D78" s="10" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E78" s="7">
         <f t="shared" si="8"/>
@@ -4871,13 +4851,13 @@
         <v>TRX12_RWD_Truck</v>
       </c>
       <c r="B79" s="9" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="C79" s="9" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="D79" s="10" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="E79" s="7">
         <f t="shared" si="8"/>
@@ -4900,13 +4880,13 @@
         <v>TRX21_RWD_LPW_LRL</v>
       </c>
       <c r="B80" s="9" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="C80" s="9" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="D80" s="9" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="E80" s="7">
         <f t="shared" si="8"/>
@@ -4929,13 +4909,13 @@
         <v>TRX21_RWD_LPW_HRL</v>
       </c>
       <c r="B81" s="9" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="C81" s="9" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="D81" s="9" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="E81" s="7">
         <f t="shared" si="8"/>
@@ -4958,13 +4938,13 @@
         <v>TRX21_RWD_MPW_LRL</v>
       </c>
       <c r="B82" s="9" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="C82" s="9" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="D82" s="10" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="E82" s="7">
         <f t="shared" si="8"/>
@@ -4987,13 +4967,13 @@
         <v>TRX21_RWD_MPW_HRL</v>
       </c>
       <c r="B83" s="9" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="C83" s="9" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="D83" s="10" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="E83" s="7">
         <f t="shared" si="8"/>
@@ -5016,13 +4996,13 @@
         <v>TRX21_RWD_HPW</v>
       </c>
       <c r="B84" s="9" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="C84" s="9" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="D84" s="10" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E84" s="7">
         <f t="shared" si="8"/>
@@ -5045,13 +5025,13 @@
         <v>TRX21_RWD_Truck</v>
       </c>
       <c r="B85" s="9" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="C85" s="9" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="D85" s="10" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="E85" s="7">
         <f t="shared" si="8"/>
@@ -5074,13 +5054,13 @@
         <v>TRX22_RWD_LPW_LRL</v>
       </c>
       <c r="B86" s="9" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="C86" s="9" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="D86" s="9" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="E86" s="7">
         <f t="shared" si="8"/>
@@ -5103,13 +5083,13 @@
         <v>TRX22_RWD_LPW_HRL</v>
       </c>
       <c r="B87" s="9" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="C87" s="9" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="D87" s="9" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="E87" s="7">
         <f t="shared" si="8"/>
@@ -5132,13 +5112,13 @@
         <v>TRX22_RWD_MPW_LRL</v>
       </c>
       <c r="B88" s="9" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="C88" s="9" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="D88" s="10" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="E88" s="7">
         <f t="shared" si="8"/>
@@ -5161,13 +5141,13 @@
         <v>TRX22_RWD_MPW_HRL</v>
       </c>
       <c r="B89" s="9" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="C89" s="9" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="D89" s="10" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="E89" s="7">
         <f t="shared" si="8"/>
@@ -5190,13 +5170,13 @@
         <v>TRX22_RWD_HPW</v>
       </c>
       <c r="B90" s="9" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="C90" s="9" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="D90" s="10" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E90" s="7">
         <f t="shared" si="8"/>
@@ -5219,13 +5199,13 @@
         <v>TRX22_RWD_Truck</v>
       </c>
       <c r="B91" s="9" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="C91" s="9" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="D91" s="10" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="E91" s="7">
         <f t="shared" si="8"/>
@@ -5265,16 +5245,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="B1" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="C1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -5324,7 +5304,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B5" s="4">
         <f t="shared" si="0"/>
@@ -5339,7 +5319,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="B6" s="4">
         <f t="shared" si="0"/>
@@ -5354,7 +5334,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B7" s="4">
         <f t="shared" si="0"/>
@@ -5369,7 +5349,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B8" s="4">
         <f t="shared" si="0"/>
@@ -5384,7 +5364,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B9" s="4">
         <f t="shared" si="0"/>
@@ -5399,7 +5379,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B10" s="4">
         <f t="shared" si="0"/>
@@ -5414,7 +5394,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B11" s="4">
         <f t="shared" si="0"/>
@@ -5429,7 +5409,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B12" s="4">
         <f t="shared" si="0"/>
@@ -5444,7 +5424,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="B13" s="4">
         <f t="shared" si="0"/>
@@ -5459,7 +5439,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B14" s="4">
         <f t="shared" si="0"/>
@@ -5474,7 +5454,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B15" s="4">
         <f t="shared" si="0"/>
@@ -5489,7 +5469,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B16" s="4">
         <f t="shared" si="0"/>
@@ -5504,7 +5484,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B17" s="4">
         <f t="shared" si="0"/>
@@ -5520,7 +5500,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B18" s="4">
         <f t="shared" si="0"/>
@@ -5536,7 +5516,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B19" s="4">
         <f t="shared" si="0"/>
@@ -5552,7 +5532,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="B20" s="4">
         <f t="shared" si="0"/>
@@ -5568,7 +5548,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B21" s="4">
         <f t="shared" si="0"/>
@@ -5584,7 +5564,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B22" s="4">
         <f t="shared" si="0"/>
@@ -5620,7 +5600,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="B1" t="s">
         <v>10</v>
@@ -5629,13 +5609,13 @@
         <v>11</v>
       </c>
       <c r="D1" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="E1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -5728,13 +5708,13 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="C1" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="D1" t="s">
         <v>7</v>
@@ -5746,12 +5726,12 @@
         <v>9</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="B2" s="4">
         <f>Markup*C2</f>
@@ -5775,7 +5755,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="B3" s="4">
         <f>Markup*C3</f>
@@ -5823,13 +5803,13 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="D1" s="9" t="s">
         <v>7</v>
@@ -5841,12 +5821,12 @@
         <v>9</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="B2" s="4">
         <f>Markup*C2</f>
@@ -5870,7 +5850,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="B3" s="4">
         <f>Markup*C3</f>
@@ -5913,25 +5893,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="B1" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C1" t="s">
         <v>12</v>
       </c>
       <c r="D1" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="E1" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="F1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -5940,10 +5920,10 @@
         <v>unibody_0</v>
       </c>
       <c r="B2" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="C2" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="D2" s="5">
         <v>0</v>
@@ -5965,7 +5945,7 @@
         <v>unibody_5</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="C3" t="s">
         <v>13</v>
@@ -5990,7 +5970,7 @@
         <v>unibody_10</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="C4" t="s">
         <v>14</v>
@@ -6015,7 +5995,7 @@
         <v>unibody_15</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="C5" t="s">
         <v>15</v>
@@ -6040,7 +6020,7 @@
         <v>unibody_20</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="C6" t="s">
         <v>16</v>
@@ -6065,10 +6045,10 @@
         <v>ladder_0</v>
       </c>
       <c r="B7" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C7" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="D7" s="6">
         <v>0</v>
@@ -6090,7 +6070,7 @@
         <v>ladder_5</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C8" t="s">
         <v>13</v>
@@ -6115,7 +6095,7 @@
         <v>ladder_10</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C9" t="s">
         <v>14</v>
@@ -6140,7 +6120,7 @@
         <v>ladder_15</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C10" t="s">
         <v>15</v>
@@ -6165,7 +6145,7 @@
         <v>ladder_20</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C11" t="s">
         <v>16</v>
@@ -6209,25 +6189,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C1" t="s">
         <v>12</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="E1" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="F1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -6236,7 +6216,7 @@
         <v>LDB</v>
       </c>
       <c r="C2" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="D2" s="9">
         <v>99</v>
@@ -6259,7 +6239,7 @@
       </c>
       <c r="B3" s="5"/>
       <c r="C3" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="D3" s="5">
         <v>99</v>
@@ -6282,7 +6262,7 @@
       </c>
       <c r="B4" s="6"/>
       <c r="C4" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D4" s="6">
         <v>99</v>
@@ -6305,10 +6285,10 @@
         <v>unibody_0</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="C5" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="D5" s="6">
         <v>0</v>
@@ -6330,10 +6310,10 @@
         <v>unibody_5</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="C6" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="D6" s="6">
         <v>5</v>
@@ -6356,10 +6336,10 @@
         <v>unibody_10</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="C7" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="D7" s="6">
         <v>10</v>
@@ -6382,10 +6362,10 @@
         <v>unibody_15</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="C8" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="D8" s="6">
         <v>15</v>
@@ -6408,10 +6388,10 @@
         <v>unibody_20</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="C9" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D9" s="6">
         <v>20</v>
@@ -6434,10 +6414,10 @@
         <v>ladder_0</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="D10" s="6">
         <v>0</v>
@@ -6459,10 +6439,10 @@
         <v>ladder_5</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="D11" s="6">
         <v>5</v>
@@ -6485,10 +6465,10 @@
         <v>ladder_10</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="D12" s="6">
         <v>10</v>
@@ -6511,10 +6491,10 @@
         <v>ladder_15</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="D13" s="6">
         <v>15</v>
@@ -6537,10 +6517,10 @@
         <v>ladder_20</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D14" s="6">
         <v>20</v>
@@ -6576,21 +6556,21 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="B1" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="C1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="D1" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="B2" s="7">
         <f>C2*Markup</f>
@@ -6605,7 +6585,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="B3" s="7">
         <f>C3*Markup</f>
@@ -6625,10 +6605,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10D61237-AECC-44ED-A2C5-2BB79F456807}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6644,64 +6624,32 @@
         <v>1.5</v>
       </c>
       <c r="C1" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>168</v>
+        <v>3</v>
       </c>
       <c r="B2" s="1">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="C2" s="1">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>169</v>
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="9" t="s">
+        <v>227</v>
       </c>
       <c r="B3" s="1">
-        <v>0</v>
-      </c>
-      <c r="C3" s="1">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>170</v>
-      </c>
-      <c r="B4" s="1">
-        <v>0</v>
-      </c>
-      <c r="C4" s="1">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="1">
-        <v>1000</v>
-      </c>
-      <c r="C5" s="1">
-        <v>2012</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="9" t="s">
-        <v>230</v>
-      </c>
-      <c r="B6" s="1">
         <v>1.2</v>
       </c>
-      <c r="C6" s="1"/>
+      <c r="C3" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -6744,7 +6692,7 @@
         <v>19</v>
       </c>
       <c r="F1" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="G1" t="s">
         <v>20</v>
@@ -7167,7 +7115,7 @@
         <v>205</v>
       </c>
       <c r="B13" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="C13" t="s">
         <v>57</v>
@@ -7197,7 +7145,7 @@
         <v>13</v>
       </c>
       <c r="L13" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
     </row>
     <row r="14" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
@@ -8899,10 +8847,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44ACC5D0-181B-4F4E-94F7-26883B6AC5A8}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="A5" sqref="A5:A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8913,15 +8861,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="B2" s="1">
         <v>0.9</v>
@@ -8929,63 +8877,50 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="B3" s="1">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>280</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="9" t="s">
         <v>284</v>
       </c>
-      <c r="B4" s="1">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>285</v>
-      </c>
-      <c r="B5" s="1">
-        <v>1.5</v>
-      </c>
+      <c r="B5" s="1"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="B6" s="1"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="B7" s="1"/>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="9" t="s">
-        <v>292</v>
-      </c>
-      <c r="B8" s="1"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="9" t="s">
-        <v>293</v>
-      </c>
-      <c r="B9" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07987B69-2230-4E5F-926C-42312732B1EC}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8995,15 +8930,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="B2" s="1">
         <v>0.4</v>
@@ -9011,51 +8946,43 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="B3" s="1">
-        <v>0</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="B4" s="1">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="9" t="s">
+        <v>290</v>
+      </c>
+      <c r="B5" s="1">
         <v>0.2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="9" t="s">
-        <v>289</v>
-      </c>
-      <c r="B5" s="1">
-        <v>1.5</v>
       </c>
     </row>
     <row r="6" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
-        <v>299</v>
-      </c>
-      <c r="B6" s="1">
-        <v>0.2</v>
+        <v>287</v>
+      </c>
+      <c r="B6" s="13">
+        <f>55/45*B5</f>
+        <v>0.24444444444444446</v>
       </c>
     </row>
     <row r="7" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="B7" s="13">
-        <f>55/45*B6</f>
-        <v>0.24444444444444446</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="9" t="s">
-        <v>295</v>
-      </c>
-      <c r="B8" s="13">
-        <f>45/55*B6</f>
+        <f>45/55*B5</f>
         <v>0.16363636363636366</v>
       </c>
     </row>
@@ -9067,10 +8994,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D89349C-4881-488D-B8C5-0F08759EC631}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:F2"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9084,27 +9011,27 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="B1" s="16" t="s">
+        <v>271</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>272</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>273</v>
+      </c>
+      <c r="E1" s="16" t="s">
         <v>274</v>
       </c>
-      <c r="C1" s="16" t="s">
-        <v>275</v>
-      </c>
-      <c r="D1" s="16" t="s">
-        <v>276</v>
-      </c>
-      <c r="E1" s="16" t="s">
-        <v>277</v>
-      </c>
       <c r="F1" s="16" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
-        <v>312</v>
+        <v>303</v>
       </c>
       <c r="B2" s="1">
         <v>0</v>
@@ -9124,7 +9051,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="B3" s="1">
         <v>-9.556E-5</v>
@@ -9144,41 +9071,21 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>279</v>
+        <v>289</v>
       </c>
       <c r="B4" s="1">
-        <v>0</v>
+        <v>8.4699999999999997E-8</v>
       </c>
       <c r="C4" s="1">
-        <v>0</v>
+        <v>-2.4901100000000001E-5</v>
       </c>
       <c r="D4" s="1">
-        <v>0</v>
+        <v>2.3686407999999998E-3</v>
       </c>
       <c r="E4" s="1">
-        <v>30</v>
+        <v>0.1245668155</v>
       </c>
       <c r="F4" s="1">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>298</v>
-      </c>
-      <c r="B5" s="1">
-        <v>8.4699999999999997E-8</v>
-      </c>
-      <c r="C5" s="1">
-        <v>-2.4901100000000001E-5</v>
-      </c>
-      <c r="D5" s="1">
-        <v>2.3686407999999998E-3</v>
-      </c>
-      <c r="E5" s="1">
-        <v>0.1245668155</v>
-      </c>
-      <c r="F5" s="1">
         <v>0</v>
       </c>
     </row>
@@ -9193,8 +9100,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D16EAC8-38E2-4645-A6B8-8BBE98EEE76B}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:F2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9209,28 +9116,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>211</v>
+      <c r="A1" s="15" t="s">
+        <v>208</v>
       </c>
       <c r="B1" s="15" t="s">
+        <v>271</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>272</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>273</v>
+      </c>
+      <c r="E1" s="15" t="s">
         <v>274</v>
       </c>
-      <c r="C1" s="14" t="s">
-        <v>275</v>
-      </c>
-      <c r="D1" s="15" t="s">
-        <v>276</v>
-      </c>
-      <c r="E1" t="s">
-        <v>277</v>
-      </c>
       <c r="F1" s="15" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>312</v>
+      <c r="A2" s="15" t="s">
+        <v>303</v>
       </c>
       <c r="B2" s="1">
         <v>0</v>
@@ -9248,9 +9155,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>296</v>
+    <row r="3" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="15" t="s">
+        <v>320</v>
       </c>
       <c r="B3" s="1">
         <v>0</v>
@@ -9269,8 +9176,8 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>297</v>
+      <c r="A4" s="15" t="s">
+        <v>321</v>
       </c>
       <c r="B4" s="1">
         <v>0</v>
@@ -9289,8 +9196,8 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>298</v>
+      <c r="A5" s="15" t="s">
+        <v>289</v>
       </c>
       <c r="B5" s="1">
         <v>0</v>
@@ -9309,8 +9216,8 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>278</v>
+      <c r="A6" s="15" t="s">
+        <v>275</v>
       </c>
       <c r="B6" s="1">
         <v>0</v>
@@ -9330,6 +9237,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -9338,7 +9246,7 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="A2" sqref="A2:A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9352,27 +9260,27 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="15" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>307</v>
+        <v>298</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>300</v>
+        <v>291</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>301</v>
+        <v>292</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>308</v>
+        <v>299</v>
       </c>
       <c r="F1" s="15" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
-        <v>313</v>
+        <v>304</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
@@ -9384,7 +9292,7 @@
         <v>0</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>324</v>
+        <v>315</v>
       </c>
       <c r="F2" s="1">
         <v>2019</v>
@@ -9392,7 +9300,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
-        <v>314</v>
+        <v>305</v>
       </c>
       <c r="B3" s="1">
         <v>1</v>
@@ -9404,7 +9312,7 @@
         <v>0</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>324</v>
+        <v>315</v>
       </c>
       <c r="F3" s="1">
         <v>2019</v>
@@ -9412,7 +9320,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="15" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="B4" s="1">
         <v>0</v>
@@ -9430,7 +9338,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="15" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="B5" s="1">
         <v>0</v>
@@ -9448,7 +9356,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="15" t="s">
-        <v>309</v>
+        <v>300</v>
       </c>
       <c r="B6" s="1">
         <v>1</v>
@@ -9460,7 +9368,7 @@
         <v>0</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>325</v>
+        <v>316</v>
       </c>
       <c r="F6" s="1">
         <v>2019</v>
@@ -9468,7 +9376,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="15" t="s">
-        <v>310</v>
+        <v>301</v>
       </c>
       <c r="B7" s="1">
         <v>1</v>
@@ -9480,7 +9388,7 @@
         <v>161.5</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>304</v>
+        <v>295</v>
       </c>
       <c r="F7" s="1">
         <v>2019</v>
@@ -9488,7 +9396,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="15" t="s">
-        <v>311</v>
+        <v>302</v>
       </c>
       <c r="B8" s="1">
         <v>1</v>
@@ -9500,7 +9408,7 @@
         <v>51</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>304</v>
+        <v>295</v>
       </c>
       <c r="F8" s="1">
         <v>2019</v>
@@ -9508,7 +9416,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="15" t="s">
-        <v>305</v>
+        <v>296</v>
       </c>
       <c r="B9" s="1">
         <v>1</v>
@@ -9520,7 +9428,7 @@
         <v>195.5</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>304</v>
+        <v>295</v>
       </c>
       <c r="F9" s="1">
         <v>2019</v>
@@ -9528,7 +9436,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="15" t="s">
-        <v>317</v>
+        <v>308</v>
       </c>
       <c r="B10" s="1">
         <v>1</v>
@@ -9540,7 +9448,7 @@
         <v>410</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>306</v>
+        <v>297</v>
       </c>
       <c r="F10" s="1">
         <v>2019</v>
@@ -9548,7 +9456,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="15" t="s">
-        <v>318</v>
+        <v>309</v>
       </c>
       <c r="B11" s="1">
         <v>1</v>
@@ -9560,7 +9468,7 @@
         <v>300</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>306</v>
+        <v>297</v>
       </c>
       <c r="F11" s="1">
         <v>2019</v>
@@ -9568,7 +9476,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="15" t="s">
-        <v>323</v>
+        <v>314</v>
       </c>
       <c r="B12" s="1">
         <v>1</v>
@@ -9580,7 +9488,7 @@
         <v>200</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>306</v>
+        <v>297</v>
       </c>
       <c r="F12" s="1">
         <v>2019</v>
@@ -9588,7 +9496,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="15" t="s">
-        <v>319</v>
+        <v>310</v>
       </c>
       <c r="B13" s="1">
         <v>1</v>
@@ -9600,7 +9508,7 @@
         <v>160</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>306</v>
+        <v>297</v>
       </c>
       <c r="F13" s="1">
         <v>2019</v>
@@ -9608,7 +9516,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="15" t="s">
-        <v>320</v>
+        <v>311</v>
       </c>
       <c r="B14" s="1">
         <v>1</v>
@@ -9620,7 +9528,7 @@
         <v>720</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>306</v>
+        <v>297</v>
       </c>
       <c r="F14" s="1">
         <v>2019</v>
@@ -9628,7 +9536,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="15" t="s">
-        <v>322</v>
+        <v>313</v>
       </c>
       <c r="B15" s="1">
         <v>0</v>
@@ -9646,7 +9554,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="15" t="s">
-        <v>321</v>
+        <v>312</v>
       </c>
       <c r="B16" s="1">
         <v>0</v>
@@ -9664,7 +9572,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -9687,27 +9596,27 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="15" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>307</v>
+        <v>298</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>300</v>
+        <v>291</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>301</v>
+        <v>292</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>308</v>
+        <v>299</v>
       </c>
       <c r="F1" s="15" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
-        <v>313</v>
+        <v>304</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
@@ -9719,7 +9628,7 @@
         <v>0</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>326</v>
+        <v>317</v>
       </c>
       <c r="F2" s="1">
         <v>2019</v>
@@ -9727,7 +9636,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
-        <v>314</v>
+        <v>305</v>
       </c>
       <c r="B3" s="1">
         <v>1</v>
@@ -9739,7 +9648,7 @@
         <v>0</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>326</v>
+        <v>317</v>
       </c>
       <c r="F3" s="1">
         <v>2019</v>
@@ -9747,7 +9656,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="15" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="B4" s="1">
         <v>1</v>
@@ -9759,7 +9668,7 @@
         <v>0</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>326</v>
+        <v>317</v>
       </c>
       <c r="F4" s="1">
         <v>0</v>
@@ -9767,7 +9676,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="15" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="B5" s="1">
         <v>1</v>
@@ -9779,7 +9688,7 @@
         <v>0</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>326</v>
+        <v>317</v>
       </c>
       <c r="F5" s="1">
         <v>0</v>
@@ -9787,7 +9696,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="15" t="s">
-        <v>309</v>
+        <v>300</v>
       </c>
       <c r="B6" s="1">
         <v>1</v>
@@ -9799,7 +9708,7 @@
         <v>0</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>325</v>
+        <v>316</v>
       </c>
       <c r="F6" s="1">
         <v>2019</v>
@@ -9807,7 +9716,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="15" t="s">
-        <v>310</v>
+        <v>301</v>
       </c>
       <c r="B7" s="1">
         <v>1</v>
@@ -9819,7 +9728,7 @@
         <v>161.5</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>304</v>
+        <v>295</v>
       </c>
       <c r="F7" s="1">
         <v>2019</v>
@@ -9827,7 +9736,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="15" t="s">
-        <v>311</v>
+        <v>302</v>
       </c>
       <c r="B8" s="1">
         <v>1</v>
@@ -9839,7 +9748,7 @@
         <v>51</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>304</v>
+        <v>295</v>
       </c>
       <c r="F8" s="1">
         <v>2019</v>
@@ -9847,7 +9756,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="15" t="s">
-        <v>305</v>
+        <v>296</v>
       </c>
       <c r="B9" s="1">
         <v>1</v>
@@ -9859,7 +9768,7 @@
         <v>195.5</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>304</v>
+        <v>295</v>
       </c>
       <c r="F9" s="1">
         <v>2019</v>
@@ -9867,7 +9776,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="15" t="s">
-        <v>317</v>
+        <v>308</v>
       </c>
       <c r="B10" s="1">
         <v>2</v>
@@ -9879,7 +9788,7 @@
         <v>410</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>306</v>
+        <v>297</v>
       </c>
       <c r="F10" s="1">
         <v>2019</v>
@@ -9887,7 +9796,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="15" t="s">
-        <v>318</v>
+        <v>309</v>
       </c>
       <c r="B11" s="1">
         <v>2</v>
@@ -9899,7 +9808,7 @@
         <v>300</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>306</v>
+        <v>297</v>
       </c>
       <c r="F11" s="1">
         <v>2019</v>
@@ -9907,7 +9816,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="15" t="s">
-        <v>323</v>
+        <v>314</v>
       </c>
       <c r="B12" s="1">
         <v>1</v>
@@ -9919,7 +9828,7 @@
         <v>200</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>306</v>
+        <v>297</v>
       </c>
       <c r="F12" s="1">
         <v>2019</v>
@@ -9927,7 +9836,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="15" t="s">
-        <v>319</v>
+        <v>310</v>
       </c>
       <c r="B13" s="1">
         <v>1</v>
@@ -9939,7 +9848,7 @@
         <v>160</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>306</v>
+        <v>297</v>
       </c>
       <c r="F13" s="1">
         <v>2019</v>
@@ -9947,7 +9856,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="15" t="s">
-        <v>320</v>
+        <v>311</v>
       </c>
       <c r="B14" s="1">
         <v>1</v>
@@ -9959,7 +9868,7 @@
         <v>720</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>306</v>
+        <v>297</v>
       </c>
       <c r="F14" s="1">
         <v>2019</v>
@@ -9967,7 +9876,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="15" t="s">
-        <v>322</v>
+        <v>313</v>
       </c>
       <c r="B15" s="1">
         <v>0</v>
@@ -9985,7 +9894,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="15" t="s">
-        <v>321</v>
+        <v>312</v>
       </c>
       <c r="B16" s="1">
         <v>1</v>
@@ -9997,7 +9906,7 @@
         <v>190</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>306</v>
+        <v>297</v>
       </c>
       <c r="F16" s="1">
         <v>0</v>
@@ -10026,27 +9935,27 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="B1" t="s">
-        <v>307</v>
+        <v>298</v>
       </c>
       <c r="C1" t="s">
-        <v>300</v>
+        <v>291</v>
       </c>
       <c r="D1" t="s">
-        <v>301</v>
+        <v>292</v>
       </c>
       <c r="E1" t="s">
-        <v>308</v>
+        <v>299</v>
       </c>
       <c r="F1" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>313</v>
+        <v>304</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
@@ -10058,7 +9967,7 @@
         <v>-8.64</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>302</v>
+        <v>293</v>
       </c>
       <c r="F2" s="1">
         <v>2019</v>
@@ -10066,7 +9975,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>314</v>
+        <v>305</v>
       </c>
       <c r="B3" s="1">
         <v>1</v>
@@ -10078,7 +9987,7 @@
         <v>231</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>302</v>
+        <v>293</v>
       </c>
       <c r="F3" s="1">
         <v>2019</v>
@@ -10086,7 +9995,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="B4" s="1">
         <v>0</v>
@@ -10104,7 +10013,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="B5" s="1">
         <v>0</v>
@@ -10122,7 +10031,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>309</v>
+        <v>300</v>
       </c>
       <c r="B6" s="1">
         <v>1</v>
@@ -10134,7 +10043,7 @@
         <v>0</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>303</v>
+        <v>294</v>
       </c>
       <c r="F6" s="1">
         <v>2019</v>
@@ -10142,7 +10051,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>310</v>
+        <v>301</v>
       </c>
       <c r="B7" s="1">
         <v>1</v>
@@ -10154,7 +10063,7 @@
         <v>161.5</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>304</v>
+        <v>295</v>
       </c>
       <c r="F7" s="1">
         <v>2019</v>
@@ -10162,7 +10071,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>311</v>
+        <v>302</v>
       </c>
       <c r="B8" s="1">
         <v>1</v>
@@ -10174,7 +10083,7 @@
         <v>51</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>304</v>
+        <v>295</v>
       </c>
       <c r="F8" s="1">
         <v>2019</v>
@@ -10182,7 +10091,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>305</v>
+        <v>296</v>
       </c>
       <c r="B9" s="1">
         <v>1</v>
@@ -10194,7 +10103,7 @@
         <v>195.5</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>304</v>
+        <v>295</v>
       </c>
       <c r="F9" s="1">
         <v>2019</v>
@@ -10202,7 +10111,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>317</v>
+        <v>308</v>
       </c>
       <c r="B10" s="1">
         <v>0</v>
@@ -10220,7 +10129,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>318</v>
+        <v>309</v>
       </c>
       <c r="B11" s="1">
         <v>0</v>
@@ -10238,7 +10147,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>323</v>
+        <v>314</v>
       </c>
       <c r="B12" s="1">
         <v>0</v>
@@ -10256,7 +10165,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>319</v>
+        <v>310</v>
       </c>
       <c r="B13" s="1">
         <v>0</v>
@@ -10274,7 +10183,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>320</v>
+        <v>311</v>
       </c>
       <c r="B14" s="1">
         <v>0</v>
@@ -10292,7 +10201,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>322</v>
+        <v>313</v>
       </c>
       <c r="B15" s="1">
         <v>1</v>
@@ -10304,7 +10213,7 @@
         <v>200</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>306</v>
+        <v>297</v>
       </c>
       <c r="F15" s="1">
         <v>2019</v>
@@ -10312,7 +10221,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>321</v>
+        <v>312</v>
       </c>
       <c r="B16" s="1">
         <v>0</v>

</xml_diff>

<commit_message>
Continue alpha_package_costs.py documentation. Updates to alpha_package_costs_module_inputs.xlsx file (no changes to any results).
</commit_message>
<xml_diff>
--- a/omega_preproc/alpha_package_costs/inputs/alpha_package_costs_module_inputs.xlsx
+++ b/omega_preproc/alpha_package_costs/inputs/alpha_package_costs_module_inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TSHERWOO\PycharmProjects\EPA_OMEGA_Model\omega_preproc\alpha_package_costs\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22CC0815-3A9B-44C7-A73F-A9595F15F506}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{741D536E-C4E7-4C1A-B262-8F3F72A82DF2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="826" xr2:uid="{31AE0ECC-ADD6-46A3-9F50-4BA6582DDF8B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="826" activeTab="8" xr2:uid="{31AE0ECC-ADD6-46A3-9F50-4BA6582DDF8B}"/>
   </bookViews>
   <sheets>
     <sheet name="inputs_code" sheetId="15" r:id="rId1"/>
@@ -39,11 +39,11 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="17" hidden="1">nonaero!$C$1:$E$4</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">trans!$A$1:$H$91</definedName>
     <definedName name="AWD_scaler">inputs_workbook!$B$3</definedName>
-    <definedName name="Markup">inputs_workbook!$B$1</definedName>
+    <definedName name="Markup">inputs_workbook!$B$2</definedName>
     <definedName name="Null_4cyl_DMC">inputs_workbook!#REF!</definedName>
     <definedName name="Null_6cyl_DMC">inputs_workbook!#REF!</definedName>
     <definedName name="Null_8cyl_DMC">inputs_workbook!#REF!</definedName>
-    <definedName name="TRX10_">inputs_workbook!$B$2</definedName>
+    <definedName name="TRX10_">inputs_workbook!#REF!</definedName>
     <definedName name="workbook_dollar_basis">inputs_workbook!#REF!</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -317,7 +317,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="948" uniqueCount="322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="952" uniqueCount="324">
   <si>
     <t>Markup</t>
   </si>
@@ -1219,9 +1219,6 @@
     <t>scale_by</t>
   </si>
   <si>
-    <t>DCDC_converter</t>
-  </si>
-  <si>
     <t>HV_orange_cables</t>
   </si>
   <si>
@@ -1283,6 +1280,15 @@
   </si>
   <si>
     <t>dollar_basis_for_output_file</t>
+  </si>
+  <si>
+    <t>kW value to be added to OBC kW value</t>
+  </si>
+  <si>
+    <t>OBC_and_DCDC_converter</t>
+  </si>
+  <si>
+    <t>kW value</t>
   </si>
 </sst>
 </file>
@@ -1949,7 +1955,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF58B9CD-C45C-4464-97D6-845ECC18E560}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
@@ -1983,7 +1989,7 @@
     </row>
     <row r="4" spans="1:2" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="15" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B4" s="1">
         <v>2020</v>
@@ -2531,7 +2537,7 @@
     </row>
     <row r="28" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="15" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B28" s="7">
         <f t="shared" si="1"/>
@@ -2613,8 +2619,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24394527-83C9-43E1-99B9-F6C50D02F0E0}">
   <dimension ref="A1:H91"/>
   <sheetViews>
-    <sheetView topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5267,7 +5273,7 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A20" sqref="A20:A22"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5916,7 +5922,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:G11"/>
+      <selection sqref="A1:G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6209,7 +6215,7 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5:G14"/>
+      <selection sqref="A1:G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6581,9 +6587,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A4F4307-4CCE-4E39-8D04-CE4F082A04BF}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -6638,10 +6642,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10D61237-AECC-44ED-A2C5-2BB79F456807}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6649,36 +6653,29 @@
     <col min="1" max="1" width="20.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3">
+    <row r="1" spans="1:2" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="15" t="s">
+        <v>208</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3">
         <v>1.5</v>
       </c>
-      <c r="C1" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="1">
-        <v>1000</v>
-      </c>
-      <c r="C2" s="1">
-        <v>2012</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
         <v>227</v>
       </c>
       <c r="B3" s="1">
         <v>1.2</v>
       </c>
-      <c r="C3" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8883,7 +8880,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:A7"/>
+      <selection sqref="A1:A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8953,7 +8950,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9027,10 +9024,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D89349C-4881-488D-B8C5-0F08759EC631}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9062,63 +9059,43 @@
         <v>217</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="15" t="s">
-        <v>303</v>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>275</v>
       </c>
       <c r="B2" s="1">
-        <v>0</v>
+        <v>-9.556E-5</v>
       </c>
       <c r="C2" s="1">
-        <v>0</v>
+        <v>2.652171E-2</v>
       </c>
       <c r="D2" s="1">
-        <v>0</v>
+        <v>-2.5608517599999998</v>
       </c>
       <c r="E2" s="1">
-        <v>3.5</v>
+        <v>193.19055123999999</v>
       </c>
       <c r="F2" s="1">
-        <v>0</v>
+        <v>2019</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>275</v>
+        <v>289</v>
       </c>
       <c r="B3" s="1">
-        <v>-9.556E-5</v>
+        <v>8.4699999999999997E-8</v>
       </c>
       <c r="C3" s="1">
-        <v>2.652171E-2</v>
+        <v>-2.4901100000000001E-5</v>
       </c>
       <c r="D3" s="1">
-        <v>-2.5608517599999998</v>
+        <v>2.3686407999999998E-3</v>
       </c>
       <c r="E3" s="1">
-        <v>193.19055123999999</v>
+        <v>0.1245668155</v>
       </c>
       <c r="F3" s="1">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>289</v>
-      </c>
-      <c r="B4" s="1">
-        <v>8.4699999999999997E-8</v>
-      </c>
-      <c r="C4" s="1">
-        <v>-2.4901100000000001E-5</v>
-      </c>
-      <c r="D4" s="1">
-        <v>2.3686407999999998E-3</v>
-      </c>
-      <c r="E4" s="1">
-        <v>0.1245668155</v>
-      </c>
-      <c r="F4" s="1">
         <v>0</v>
       </c>
     </row>
@@ -9131,10 +9108,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D16EAC8-38E2-4645-A6B8-8BBE98EEE76B}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9168,9 +9145,9 @@
         <v>217</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
-        <v>303</v>
+        <v>318</v>
       </c>
       <c r="B2" s="1">
         <v>0</v>
@@ -9179,16 +9156,16 @@
         <v>0</v>
       </c>
       <c r="D2" s="1">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="E2" s="1">
-        <v>3.5</v>
+        <v>0.14099999999999999</v>
       </c>
       <c r="F2" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
         <v>319</v>
       </c>
@@ -9199,10 +9176,10 @@
         <v>0</v>
       </c>
       <c r="D3" s="1">
-        <v>1E-3</v>
+        <v>2.7900000000000001E-2</v>
       </c>
       <c r="E3" s="1">
-        <v>0.14099999999999999</v>
+        <v>-13.269</v>
       </c>
       <c r="F3" s="1">
         <v>0</v>
@@ -9210,7 +9187,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="15" t="s">
-        <v>320</v>
+        <v>289</v>
       </c>
       <c r="B4" s="1">
         <v>0</v>
@@ -9219,10 +9196,10 @@
         <v>0</v>
       </c>
       <c r="D4" s="1">
-        <v>2.7900000000000001E-2</v>
+        <v>1.4200000000000001E-2</v>
       </c>
       <c r="E4" s="1">
-        <v>-13.269</v>
+        <v>6.4799999999999996E-2</v>
       </c>
       <c r="F4" s="1">
         <v>0</v>
@@ -9230,7 +9207,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="15" t="s">
-        <v>289</v>
+        <v>275</v>
       </c>
       <c r="B5" s="1">
         <v>0</v>
@@ -9239,32 +9216,12 @@
         <v>0</v>
       </c>
       <c r="D5" s="1">
-        <v>1.4200000000000001E-2</v>
+        <v>-250.72</v>
       </c>
       <c r="E5" s="1">
-        <v>6.4799999999999996E-2</v>
+        <v>1058.2</v>
       </c>
       <c r="F5" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="15" t="s">
-        <v>275</v>
-      </c>
-      <c r="B6" s="1">
-        <v>0</v>
-      </c>
-      <c r="C6" s="1">
-        <v>0</v>
-      </c>
-      <c r="D6" s="1">
-        <v>-250.72</v>
-      </c>
-      <c r="E6" s="1">
-        <v>1058.2</v>
-      </c>
-      <c r="F6" s="1">
         <v>2017</v>
       </c>
     </row>
@@ -9276,17 +9233,17 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D1A1908-ADF0-4823-836D-799AF3E6FC99}">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A16"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="32.6640625" style="15" bestFit="1" customWidth="1"/>
     <col min="2" max="4" width="8.88671875" style="15"/>
-    <col min="5" max="5" width="21.5546875" style="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33.21875" style="15" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.6640625" style="15" bestFit="1" customWidth="1"/>
     <col min="7" max="16384" width="8.88671875" style="15"/>
   </cols>
@@ -9313,7 +9270,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
@@ -9325,7 +9282,7 @@
         <v>0</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="F2" s="1">
         <v>2019</v>
@@ -9333,7 +9290,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B3" s="1">
         <v>1</v>
@@ -9345,7 +9302,7 @@
         <v>0</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="F3" s="1">
         <v>2019</v>
@@ -9353,7 +9310,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="15" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B4" s="1">
         <v>0</v>
@@ -9371,7 +9328,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="15" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B5" s="1">
         <v>0</v>
@@ -9388,40 +9345,40 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="15" t="s">
-        <v>300</v>
+      <c r="A6" s="10" t="s">
+        <v>302</v>
       </c>
       <c r="B6" s="1">
         <v>1</v>
       </c>
       <c r="C6" s="1">
-        <v>39.753793103448274</v>
+        <v>0</v>
       </c>
       <c r="D6" s="1">
-        <v>0</v>
+        <v>3.5</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>316</v>
+        <v>321</v>
       </c>
       <c r="F6" s="1">
-        <v>2019</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="15" t="s">
-        <v>301</v>
+        <v>322</v>
       </c>
       <c r="B7" s="1">
         <v>1</v>
       </c>
       <c r="C7" s="1">
-        <v>9.5</v>
+        <v>39.753793103448274</v>
       </c>
       <c r="D7" s="1">
-        <v>161.5</v>
+        <v>0</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>295</v>
+        <v>315</v>
       </c>
       <c r="F7" s="1">
         <v>2019</v>
@@ -9429,16 +9386,16 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="15" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B8" s="1">
         <v>1</v>
       </c>
       <c r="C8" s="1">
-        <v>3</v>
+        <v>9.5</v>
       </c>
       <c r="D8" s="1">
-        <v>51</v>
+        <v>161.5</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>295</v>
@@ -9449,16 +9406,16 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="15" t="s">
-        <v>296</v>
+        <v>301</v>
       </c>
       <c r="B9" s="1">
         <v>1</v>
       </c>
       <c r="C9" s="1">
-        <v>11.5</v>
+        <v>3</v>
       </c>
       <c r="D9" s="1">
-        <v>195.5</v>
+        <v>51</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>295</v>
@@ -9469,19 +9426,19 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="15" t="s">
-        <v>308</v>
+        <v>296</v>
       </c>
       <c r="B10" s="1">
         <v>1</v>
       </c>
       <c r="C10" s="1">
-        <v>0</v>
+        <v>11.5</v>
       </c>
       <c r="D10" s="1">
-        <v>410</v>
+        <v>195.5</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="F10" s="1">
         <v>2019</v>
@@ -9489,7 +9446,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="15" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="B11" s="1">
         <v>1</v>
@@ -9498,7 +9455,7 @@
         <v>0</v>
       </c>
       <c r="D11" s="1">
-        <v>300</v>
+        <v>410</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>297</v>
@@ -9509,7 +9466,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="15" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
       <c r="B12" s="1">
         <v>1</v>
@@ -9518,7 +9475,7 @@
         <v>0</v>
       </c>
       <c r="D12" s="1">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>297</v>
@@ -9529,7 +9486,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="15" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="B13" s="1">
         <v>1</v>
@@ -9538,7 +9495,7 @@
         <v>0</v>
       </c>
       <c r="D13" s="1">
-        <v>160</v>
+        <v>200</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>297</v>
@@ -9549,7 +9506,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="15" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="B14" s="1">
         <v>1</v>
@@ -9558,7 +9515,7 @@
         <v>0</v>
       </c>
       <c r="D14" s="1">
-        <v>720</v>
+        <v>160</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>297</v>
@@ -9569,20 +9526,22 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="15" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="B15" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C15" s="1">
         <v>0</v>
       </c>
       <c r="D15" s="1">
-        <v>0</v>
-      </c>
-      <c r="E15" s="1"/>
+        <v>720</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>297</v>
+      </c>
       <c r="F15" s="1">
-        <v>0</v>
+        <v>2019</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -9600,6 +9559,24 @@
       </c>
       <c r="E16" s="1"/>
       <c r="F16" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="15" t="s">
+        <v>311</v>
+      </c>
+      <c r="B17" s="1">
+        <v>0</v>
+      </c>
+      <c r="C17" s="1">
+        <v>0</v>
+      </c>
+      <c r="D17" s="1">
+        <v>0</v>
+      </c>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1">
         <v>0</v>
       </c>
     </row>
@@ -9612,17 +9589,17 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4932C69-09AA-44A9-AC5E-22F05F727E1B}">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A16"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="32.6640625" style="15" bestFit="1" customWidth="1"/>
     <col min="2" max="4" width="8.88671875" style="15"/>
-    <col min="5" max="5" width="21.5546875" style="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33.21875" style="15" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.6640625" style="15" bestFit="1" customWidth="1"/>
     <col min="7" max="16384" width="8.88671875" style="15"/>
   </cols>
@@ -9649,7 +9626,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
@@ -9661,7 +9638,7 @@
         <v>0</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="F2" s="1">
         <v>2019</v>
@@ -9669,7 +9646,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B3" s="1">
         <v>1</v>
@@ -9681,7 +9658,7 @@
         <v>0</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="F3" s="1">
         <v>2019</v>
@@ -9689,7 +9666,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="15" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B4" s="1">
         <v>1</v>
@@ -9701,7 +9678,7 @@
         <v>0</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="F4" s="1">
         <v>0</v>
@@ -9709,7 +9686,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="15" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B5" s="1">
         <v>1</v>
@@ -9721,47 +9698,47 @@
         <v>0</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="F5" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="15" t="s">
-        <v>300</v>
+      <c r="A6" s="10" t="s">
+        <v>302</v>
       </c>
       <c r="B6" s="1">
         <v>1</v>
       </c>
       <c r="C6" s="1">
-        <v>39.753793103448274</v>
+        <v>0</v>
       </c>
       <c r="D6" s="1">
-        <v>0</v>
+        <v>3.5</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>316</v>
+        <v>321</v>
       </c>
       <c r="F6" s="1">
-        <v>2019</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="15" t="s">
-        <v>301</v>
+        <v>322</v>
       </c>
       <c r="B7" s="1">
         <v>1</v>
       </c>
       <c r="C7" s="1">
-        <v>9.5</v>
+        <v>39.753793103448274</v>
       </c>
       <c r="D7" s="1">
-        <v>161.5</v>
+        <v>0</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>295</v>
+        <v>315</v>
       </c>
       <c r="F7" s="1">
         <v>2019</v>
@@ -9769,16 +9746,16 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="15" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B8" s="1">
         <v>1</v>
       </c>
       <c r="C8" s="1">
-        <v>3</v>
+        <v>9.5</v>
       </c>
       <c r="D8" s="1">
-        <v>51</v>
+        <v>161.5</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>295</v>
@@ -9789,16 +9766,16 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="15" t="s">
-        <v>296</v>
+        <v>301</v>
       </c>
       <c r="B9" s="1">
         <v>1</v>
       </c>
       <c r="C9" s="1">
-        <v>11.5</v>
+        <v>3</v>
       </c>
       <c r="D9" s="1">
-        <v>195.5</v>
+        <v>51</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>295</v>
@@ -9809,19 +9786,19 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="15" t="s">
-        <v>308</v>
+        <v>296</v>
       </c>
       <c r="B10" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C10" s="1">
-        <v>0</v>
+        <v>11.5</v>
       </c>
       <c r="D10" s="1">
-        <v>410</v>
+        <v>195.5</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="F10" s="1">
         <v>2019</v>
@@ -9829,7 +9806,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="15" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="B11" s="1">
         <v>2</v>
@@ -9838,7 +9815,7 @@
         <v>0</v>
       </c>
       <c r="D11" s="1">
-        <v>300</v>
+        <v>410</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>297</v>
@@ -9849,16 +9826,16 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="15" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
       <c r="B12" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C12" s="1">
         <v>0</v>
       </c>
       <c r="D12" s="1">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>297</v>
@@ -9869,7 +9846,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="15" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="B13" s="1">
         <v>1</v>
@@ -9878,7 +9855,7 @@
         <v>0</v>
       </c>
       <c r="D13" s="1">
-        <v>160</v>
+        <v>200</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>297</v>
@@ -9889,7 +9866,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="15" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="B14" s="1">
         <v>1</v>
@@ -9898,7 +9875,7 @@
         <v>0</v>
       </c>
       <c r="D14" s="1">
-        <v>720</v>
+        <v>160</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>297</v>
@@ -9909,20 +9886,22 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="15" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="B15" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C15" s="1">
         <v>0</v>
       </c>
       <c r="D15" s="1">
-        <v>0</v>
-      </c>
-      <c r="E15" s="1"/>
+        <v>720</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>297</v>
+      </c>
       <c r="F15" s="1">
-        <v>0</v>
+        <v>2019</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -9930,18 +9909,36 @@
         <v>312</v>
       </c>
       <c r="B16" s="1">
+        <v>0</v>
+      </c>
+      <c r="C16" s="1">
+        <v>0</v>
+      </c>
+      <c r="D16" s="1">
+        <v>0</v>
+      </c>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="15" t="s">
+        <v>311</v>
+      </c>
+      <c r="B17" s="1">
         <v>1</v>
       </c>
-      <c r="C16" s="1">
-        <v>0</v>
-      </c>
-      <c r="D16" s="1">
+      <c r="C17" s="1">
+        <v>0</v>
+      </c>
+      <c r="D17" s="1">
         <v>190</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="E17" s="1" t="s">
         <v>297</v>
       </c>
-      <c r="F16" s="1">
+      <c r="F17" s="1">
         <v>0</v>
       </c>
     </row>
@@ -9953,16 +9950,16 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{705C8F8E-56DC-45B6-9939-45B902DFD251}">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="32.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33.21875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -9988,7 +9985,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
@@ -10008,7 +10005,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B3" s="1">
         <v>1</v>
@@ -10028,7 +10025,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B4" s="1">
         <v>0</v>
@@ -10046,7 +10043,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B5" s="1">
         <v>0</v>
@@ -10062,41 +10059,41 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>300</v>
+    <row r="6" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="10" t="s">
+        <v>302</v>
       </c>
       <c r="B6" s="1">
         <v>1</v>
       </c>
       <c r="C6" s="1">
-        <v>39.753793103448274</v>
+        <v>0</v>
       </c>
       <c r="D6" s="1">
-        <v>0</v>
+        <v>3.5</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>294</v>
+        <v>323</v>
       </c>
       <c r="F6" s="1">
-        <v>2019</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>301</v>
+        <v>322</v>
       </c>
       <c r="B7" s="1">
         <v>1</v>
       </c>
       <c r="C7" s="1">
-        <v>9.5</v>
+        <v>39.753793103448274</v>
       </c>
       <c r="D7" s="1">
-        <v>161.5</v>
+        <v>0</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="F7" s="1">
         <v>2019</v>
@@ -10104,16 +10101,16 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B8" s="1">
         <v>1</v>
       </c>
       <c r="C8" s="1">
-        <v>3</v>
+        <v>9.5</v>
       </c>
       <c r="D8" s="1">
-        <v>51</v>
+        <v>161.5</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>295</v>
@@ -10124,16 +10121,16 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>296</v>
+        <v>301</v>
       </c>
       <c r="B9" s="1">
         <v>1</v>
       </c>
       <c r="C9" s="1">
-        <v>11.5</v>
+        <v>3</v>
       </c>
       <c r="D9" s="1">
-        <v>195.5</v>
+        <v>51</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>295</v>
@@ -10144,25 +10141,27 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>308</v>
+        <v>296</v>
       </c>
       <c r="B10" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C10" s="1">
-        <v>0</v>
+        <v>11.5</v>
       </c>
       <c r="D10" s="1">
-        <v>0</v>
-      </c>
-      <c r="E10" s="1"/>
+        <v>195.5</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>295</v>
+      </c>
       <c r="F10" s="1">
-        <v>0</v>
+        <v>2019</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="B11" s="1">
         <v>0</v>
@@ -10180,7 +10179,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
       <c r="B12" s="1">
         <v>0</v>
@@ -10198,7 +10197,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="B13" s="1">
         <v>0</v>
@@ -10216,7 +10215,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="B14" s="1">
         <v>0</v>
@@ -10234,22 +10233,20 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="B15" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C15" s="1">
         <v>0</v>
       </c>
       <c r="D15" s="1">
-        <v>200</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>297</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="E15" s="1"/>
       <c r="F15" s="1">
-        <v>2019</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -10257,16 +10254,36 @@
         <v>312</v>
       </c>
       <c r="B16" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C16" s="1">
         <v>0</v>
       </c>
       <c r="D16" s="1">
-        <v>0</v>
-      </c>
-      <c r="E16" s="1"/>
+        <v>200</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>297</v>
+      </c>
       <c r="F16" s="1">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>311</v>
+      </c>
+      <c r="B17" s="1">
+        <v>0</v>
+      </c>
+      <c r="C17" s="1">
+        <v>0</v>
+      </c>
+      <c r="D17" s="1">
+        <v>0</v>
+      </c>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Revise to piece together some PHEVs for testing.
</commit_message>
<xml_diff>
--- a/omega_preproc/alpha_package_costs/inputs/alpha_package_costs_module_inputs.xlsx
+++ b/omega_preproc/alpha_package_costs/inputs/alpha_package_costs_module_inputs.xlsx
@@ -8,36 +8,40 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TSHERWOO\PycharmProjects\EPA_OMEGA_Model\omega_preproc\alpha_package_costs\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{741D536E-C4E7-4C1A-B262-8F3F72A82DF2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6092E0B-E234-4D7B-8226-AEDDA1BBF603}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="826" activeTab="8" xr2:uid="{31AE0ECC-ADD6-46A3-9F50-4BA6582DDF8B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="826" xr2:uid="{31AE0ECC-ADD6-46A3-9F50-4BA6582DDF8B}"/>
   </bookViews>
   <sheets>
     <sheet name="inputs_code" sheetId="15" r:id="rId1"/>
     <sheet name="inputs_workbook" sheetId="8" r:id="rId2"/>
-    <sheet name="pev_metrics" sheetId="20" r:id="rId3"/>
-    <sheet name="hev_metrics" sheetId="24" r:id="rId4"/>
-    <sheet name="bev_curves" sheetId="21" r:id="rId5"/>
-    <sheet name="hev_curves" sheetId="23" r:id="rId6"/>
-    <sheet name="bev_nonbattery_single" sheetId="26" r:id="rId7"/>
-    <sheet name="bev_nonbattery_dual" sheetId="27" r:id="rId8"/>
-    <sheet name="hev_nonbattery" sheetId="25" r:id="rId9"/>
-    <sheet name="price_class" sheetId="19" r:id="rId10"/>
-    <sheet name="engine" sheetId="18" r:id="rId11"/>
-    <sheet name="trans" sheetId="2" r:id="rId12"/>
-    <sheet name="accessories" sheetId="3" r:id="rId13"/>
-    <sheet name="start-stop" sheetId="5" r:id="rId14"/>
-    <sheet name="weight_ice" sheetId="4" r:id="rId15"/>
-    <sheet name="weight_pev" sheetId="22" r:id="rId16"/>
-    <sheet name="aero" sheetId="6" r:id="rId17"/>
-    <sheet name="nonaero" sheetId="9" r:id="rId18"/>
-    <sheet name="ac" sheetId="17" r:id="rId19"/>
-    <sheet name="et_dmc" sheetId="7" r:id="rId20"/>
+    <sheet name="bev_metrics" sheetId="20" r:id="rId3"/>
+    <sheet name="phev_metrics" sheetId="30" r:id="rId4"/>
+    <sheet name="hev_metrics" sheetId="24" r:id="rId5"/>
+    <sheet name="bev_curves" sheetId="21" r:id="rId6"/>
+    <sheet name="phev_curves" sheetId="28" r:id="rId7"/>
+    <sheet name="hev_curves" sheetId="23" r:id="rId8"/>
+    <sheet name="bev_nonbattery_single" sheetId="26" r:id="rId9"/>
+    <sheet name="bev_nonbattery_dual" sheetId="27" r:id="rId10"/>
+    <sheet name="phev_nonbattery_single" sheetId="29" r:id="rId11"/>
+    <sheet name="phev_nonbattery_dual" sheetId="31" r:id="rId12"/>
+    <sheet name="hev_nonbattery" sheetId="25" r:id="rId13"/>
+    <sheet name="price_class" sheetId="19" r:id="rId14"/>
+    <sheet name="engine" sheetId="18" r:id="rId15"/>
+    <sheet name="trans" sheetId="2" r:id="rId16"/>
+    <sheet name="accessories" sheetId="3" r:id="rId17"/>
+    <sheet name="start-stop" sheetId="5" r:id="rId18"/>
+    <sheet name="weight_ice" sheetId="4" r:id="rId19"/>
+    <sheet name="weight_bev" sheetId="22" r:id="rId20"/>
+    <sheet name="aero" sheetId="6" r:id="rId21"/>
+    <sheet name="nonaero" sheetId="9" r:id="rId22"/>
+    <sheet name="ac" sheetId="17" r:id="rId23"/>
+    <sheet name="et_dmc" sheetId="7" r:id="rId24"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="16" hidden="1">aero!$B$1:$E$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="17" hidden="1">nonaero!$C$1:$E$4</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">trans!$A$1:$H$91</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="20" hidden="1">aero!$B$1:$E$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="21" hidden="1">nonaero!$C$1:$E$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="15" hidden="1">trans!$A$1:$H$91</definedName>
     <definedName name="AWD_scaler">inputs_workbook!$B$3</definedName>
     <definedName name="Markup">inputs_workbook!$B$2</definedName>
     <definedName name="Null_4cyl_DMC">inputs_workbook!#REF!</definedName>
@@ -220,6 +224,76 @@
     <author>Sherwood, Todd</author>
   </authors>
   <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{A099C000-93C7-4959-9B67-B1C1FF159E5A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Sherwood, Todd:
+From MSa: 20210406_1732</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+For battery cost, at various annual production volumes:
+50K: $/gross kWh = -0.00011558x3 + 0.03260786x2 - 3.23269439x + 243.16460812
+125K: $/gross kWh = -0.00010551x3 + 0.02954283x2 - 2.89409681x + 218.42199600
+250K: $/gross kWh = -0.00009965x3 + 0.02776430x2 - 2.69776661x + 203.67861255
+450K: $/gross kWh = -0.00009556x3 + 0.02652171x2 - 2.56085176x + 193.19055124
+Where x is gross kWh.
+For Wh/kg (if you need that for figuring battery weight):
+Wh/kg = 0.0000000847x3 – 0.0000249011 x2 + 0.0023686408 + 0.1245668155
+Where x is gross kWh.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Cost Sensitivities (all with 450K coeffs)</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+batt_cost_low, constant = 180 (aiming for approximately 80$/kWh in 2030, from BNF study)
+                      bev learning rate = 0.04
+batt_cost_high, constant = 230 (aiming for approximately 124$/kWh in 2030, from MIT study)
+                      bev learning rate = 0.01
+batt_cost_mid, constant = 193.19055124 (as above)
+                      bev learning rate = 0.025
+As of 20220114, kWh_pack_per_kg_curbwt_curve and kW_motor_per_kg_curwt_curve entries are from the hev_curves sheet with additional factors to make more like a PHEV.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Sherwood, Todd</author>
+  </authors>
+  <commentList>
     <comment ref="A1" authorId="0" shapeId="0" xr:uid="{28DA3015-FCB1-42F2-8C6F-7DA593955D44}">
       <text>
         <r>
@@ -248,7 +322,7 @@
 </comments>
 </file>
 
-<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Sherwood, Todd</author>
@@ -282,7 +356,75 @@
 </comments>
 </file>
 
-<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Sherwood, Todd</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{D0B89EC6-6258-4353-B9BC-1B1C9D33BFBE}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Sherwood, Todd:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Costing_Guide_BEV_HEV_Draft_04_30_2021.xlsx</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments7.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Sherwood, Todd</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{34CD91EA-BADB-4C78-85F3-A7A25D0D782D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Sherwood, Todd:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Costing_Guide_BEV_HEV_Draft_04_30_2021.xlsx</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments8.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Sherwood, Todd</author>
@@ -317,7 +459,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="952" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1039" uniqueCount="319">
   <si>
     <t>Markup</t>
   </si>
@@ -1153,45 +1295,9 @@
     <t>optional_run_description</t>
   </si>
   <si>
-    <t>usable_soc_bev</t>
-  </si>
-  <si>
-    <t>gap_bev</t>
-  </si>
-  <si>
-    <t>powertrain_markup_bev</t>
-  </si>
-  <si>
-    <t>usable_soc_hev</t>
-  </si>
-  <si>
-    <t>gap_hev</t>
-  </si>
-  <si>
-    <t>powertrain_markup_hev</t>
-  </si>
-  <si>
-    <t>usable_soc_phev</t>
-  </si>
-  <si>
-    <t>gap_phev</t>
-  </si>
-  <si>
-    <t>powertrain_markup_phev</t>
-  </si>
-  <si>
-    <t>co2_reduction_city_hev</t>
-  </si>
-  <si>
-    <t>co2_reduction_hwy_hev</t>
-  </si>
-  <si>
     <t>kWh_pack_per_kg_pack_curve</t>
   </si>
   <si>
-    <t>co2_reduction_cycle_hev</t>
-  </si>
-  <si>
     <t>slope</t>
   </si>
   <si>
@@ -1289,16 +1395,38 @@
   </si>
   <si>
     <t>kW value</t>
+  </si>
+  <si>
+    <t>usable_soc</t>
+  </si>
+  <si>
+    <t>gap</t>
+  </si>
+  <si>
+    <t>powertrain_markup</t>
+  </si>
+  <si>
+    <t>co2_reduction_cycle</t>
+  </si>
+  <si>
+    <t>co2_reduction_city</t>
+  </si>
+  <si>
+    <t>co2_reduction_hwy</t>
+  </si>
+  <si>
+    <t>learning_rate_phev</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(\$* #,##0.00_);_(\$* \(#,##0.00\);_(\$* \-??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
   <fonts count="22" x14ac:knownFonts="1">
     <font>
@@ -1551,7 +1679,7 @@
     <xf numFmtId="0" fontId="16" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1575,6 +1703,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="35">
     <cellStyle name="Accent1 2" xfId="20" xr:uid="{D9FD632B-EF7F-49B6-8440-0774D2DADADB}"/>
@@ -1953,10 +2082,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF58B9CD-C45C-4464-97D6-845ECC18E560}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1989,7 +2118,7 @@
     </row>
     <row r="4" spans="1:2" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="15" t="s">
-        <v>320</v>
+        <v>308</v>
       </c>
       <c r="B4" s="1">
         <v>2020</v>
@@ -2043,11 +2172,19 @@
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="9" t="s">
+    <row r="11" spans="1:2" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="15" t="s">
+        <v>318</v>
+      </c>
+      <c r="B11" s="1">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B12" s="1">
         <v>1.2</v>
       </c>
     </row>
@@ -2059,6 +2196,1429 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4932C69-09AA-44A9-AC5E-22F05F727E1B}">
+  <dimension ref="A1:F17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="32.6640625" style="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="8.88671875" style="15"/>
+    <col min="5" max="5" width="33.21875" style="15" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.6640625" style="15" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.88671875" style="15"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="15" t="s">
+        <v>208</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>286</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>279</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>280</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>287</v>
+      </c>
+      <c r="F1" s="15" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="15" t="s">
+        <v>291</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1">
+        <v>4.29</v>
+      </c>
+      <c r="D2" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="F2" s="1">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="15" t="s">
+        <v>292</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="F3" s="1">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="15" t="s">
+        <v>293</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1">
+        <v>3.12</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="15" t="s">
+        <v>294</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1">
+        <v>4</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="10" t="s">
+        <v>290</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0</v>
+      </c>
+      <c r="D6" s="1">
+        <v>3.5</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="15" t="s">
+        <v>310</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1</v>
+      </c>
+      <c r="C7" s="1">
+        <v>39.753793103448274</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="F7" s="1">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="15" t="s">
+        <v>288</v>
+      </c>
+      <c r="B8" s="1">
+        <v>1</v>
+      </c>
+      <c r="C8" s="1">
+        <v>9.5</v>
+      </c>
+      <c r="D8" s="1">
+        <v>161.5</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="F8" s="1">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="15" t="s">
+        <v>289</v>
+      </c>
+      <c r="B9" s="1">
+        <v>1</v>
+      </c>
+      <c r="C9" s="1">
+        <v>3</v>
+      </c>
+      <c r="D9" s="1">
+        <v>51</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="F9" s="1">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="15" t="s">
+        <v>284</v>
+      </c>
+      <c r="B10" s="1">
+        <v>1</v>
+      </c>
+      <c r="C10" s="1">
+        <v>11.5</v>
+      </c>
+      <c r="D10" s="1">
+        <v>195.5</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="F10" s="1">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="15" t="s">
+        <v>295</v>
+      </c>
+      <c r="B11" s="1">
+        <v>2</v>
+      </c>
+      <c r="C11" s="1">
+        <v>0</v>
+      </c>
+      <c r="D11" s="1">
+        <v>410</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="F11" s="1">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="15" t="s">
+        <v>296</v>
+      </c>
+      <c r="B12" s="1">
+        <v>2</v>
+      </c>
+      <c r="C12" s="1">
+        <v>0</v>
+      </c>
+      <c r="D12" s="1">
+        <v>300</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="F12" s="1">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="15" t="s">
+        <v>301</v>
+      </c>
+      <c r="B13" s="1">
+        <v>1</v>
+      </c>
+      <c r="C13" s="1">
+        <v>0</v>
+      </c>
+      <c r="D13" s="1">
+        <v>200</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="F13" s="1">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="15" t="s">
+        <v>297</v>
+      </c>
+      <c r="B14" s="1">
+        <v>1</v>
+      </c>
+      <c r="C14" s="1">
+        <v>0</v>
+      </c>
+      <c r="D14" s="1">
+        <v>160</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="F14" s="1">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="15" t="s">
+        <v>298</v>
+      </c>
+      <c r="B15" s="1">
+        <v>1</v>
+      </c>
+      <c r="C15" s="1">
+        <v>0</v>
+      </c>
+      <c r="D15" s="1">
+        <v>720</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="F15" s="1">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="15" t="s">
+        <v>300</v>
+      </c>
+      <c r="B16" s="1">
+        <v>0</v>
+      </c>
+      <c r="C16" s="1">
+        <v>0</v>
+      </c>
+      <c r="D16" s="1">
+        <v>0</v>
+      </c>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="15" t="s">
+        <v>299</v>
+      </c>
+      <c r="B17" s="1">
+        <v>1</v>
+      </c>
+      <c r="C17" s="1">
+        <v>0</v>
+      </c>
+      <c r="D17" s="1">
+        <v>190</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="F17" s="1">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{905A502E-9B5F-43B7-85CF-C164FE7D0DF7}">
+  <dimension ref="A1:F17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="32.6640625" style="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="8.88671875" style="15"/>
+    <col min="5" max="5" width="33.21875" style="15" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.6640625" style="15" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.88671875" style="15"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="15" t="s">
+        <v>208</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>286</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>279</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>280</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>287</v>
+      </c>
+      <c r="F1" s="15" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="15" t="s">
+        <v>291</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1">
+        <v>4.29</v>
+      </c>
+      <c r="D2" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="F2" s="1">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="15" t="s">
+        <v>292</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="F3" s="1">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="15" t="s">
+        <v>293</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="15" t="s">
+        <v>294</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="10" t="s">
+        <v>290</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0</v>
+      </c>
+      <c r="D6" s="1">
+        <v>3.5</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="15" t="s">
+        <v>310</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1</v>
+      </c>
+      <c r="C7" s="1">
+        <v>39.753793103448274</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="F7" s="1">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="15" t="s">
+        <v>288</v>
+      </c>
+      <c r="B8" s="1">
+        <v>1</v>
+      </c>
+      <c r="C8" s="1">
+        <v>9.5</v>
+      </c>
+      <c r="D8" s="1">
+        <v>161.5</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="F8" s="1">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="15" t="s">
+        <v>289</v>
+      </c>
+      <c r="B9" s="1">
+        <v>1</v>
+      </c>
+      <c r="C9" s="1">
+        <v>3</v>
+      </c>
+      <c r="D9" s="1">
+        <v>51</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="F9" s="1">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="15" t="s">
+        <v>284</v>
+      </c>
+      <c r="B10" s="1">
+        <v>1</v>
+      </c>
+      <c r="C10" s="1">
+        <v>11.5</v>
+      </c>
+      <c r="D10" s="1">
+        <v>195.5</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="F10" s="1">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="15" t="s">
+        <v>295</v>
+      </c>
+      <c r="B11" s="1">
+        <v>1</v>
+      </c>
+      <c r="C11" s="1">
+        <v>0</v>
+      </c>
+      <c r="D11" s="1">
+        <v>410</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="F11" s="1">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="15" t="s">
+        <v>296</v>
+      </c>
+      <c r="B12" s="1">
+        <v>1</v>
+      </c>
+      <c r="C12" s="1">
+        <v>0</v>
+      </c>
+      <c r="D12" s="1">
+        <v>300</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="F12" s="1">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="15" t="s">
+        <v>301</v>
+      </c>
+      <c r="B13" s="1">
+        <v>1</v>
+      </c>
+      <c r="C13" s="1">
+        <v>0</v>
+      </c>
+      <c r="D13" s="1">
+        <v>200</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="F13" s="1">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="15" t="s">
+        <v>297</v>
+      </c>
+      <c r="B14" s="1">
+        <v>1</v>
+      </c>
+      <c r="C14" s="1">
+        <v>0</v>
+      </c>
+      <c r="D14" s="1">
+        <v>160</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="F14" s="1">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="15" t="s">
+        <v>298</v>
+      </c>
+      <c r="B15" s="1">
+        <v>1</v>
+      </c>
+      <c r="C15" s="1">
+        <v>0</v>
+      </c>
+      <c r="D15" s="1">
+        <v>720</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="F15" s="1">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="15" t="s">
+        <v>300</v>
+      </c>
+      <c r="B16" s="1">
+        <v>0</v>
+      </c>
+      <c r="C16" s="1">
+        <v>0</v>
+      </c>
+      <c r="D16" s="1">
+        <v>0</v>
+      </c>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="15" t="s">
+        <v>299</v>
+      </c>
+      <c r="B17" s="1">
+        <v>0</v>
+      </c>
+      <c r="C17" s="1">
+        <v>0</v>
+      </c>
+      <c r="D17" s="1">
+        <v>0</v>
+      </c>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C680C35-781A-42DE-8E34-DB76B75545CF}">
+  <dimension ref="A1:F17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="32.6640625" style="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="8.88671875" style="15"/>
+    <col min="5" max="5" width="33.21875" style="15" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.6640625" style="15" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.88671875" style="15"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="15" t="s">
+        <v>208</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>286</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>279</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>280</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>287</v>
+      </c>
+      <c r="F1" s="15" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="15" t="s">
+        <v>291</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1">
+        <v>4.29</v>
+      </c>
+      <c r="D2" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="F2" s="1">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="15" t="s">
+        <v>292</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="F3" s="1">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="15" t="s">
+        <v>293</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1">
+        <v>3.12</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="15" t="s">
+        <v>294</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1">
+        <v>4</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="10" t="s">
+        <v>290</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0</v>
+      </c>
+      <c r="D6" s="1">
+        <v>3.5</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="15" t="s">
+        <v>310</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1</v>
+      </c>
+      <c r="C7" s="1">
+        <v>39.753793103448274</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="F7" s="1">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="15" t="s">
+        <v>288</v>
+      </c>
+      <c r="B8" s="1">
+        <v>1</v>
+      </c>
+      <c r="C8" s="1">
+        <v>9.5</v>
+      </c>
+      <c r="D8" s="1">
+        <v>161.5</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="F8" s="1">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="15" t="s">
+        <v>289</v>
+      </c>
+      <c r="B9" s="1">
+        <v>1</v>
+      </c>
+      <c r="C9" s="1">
+        <v>3</v>
+      </c>
+      <c r="D9" s="1">
+        <v>51</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="F9" s="1">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="15" t="s">
+        <v>284</v>
+      </c>
+      <c r="B10" s="1">
+        <v>1</v>
+      </c>
+      <c r="C10" s="1">
+        <v>11.5</v>
+      </c>
+      <c r="D10" s="1">
+        <v>195.5</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="F10" s="1">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="15" t="s">
+        <v>295</v>
+      </c>
+      <c r="B11" s="1">
+        <v>2</v>
+      </c>
+      <c r="C11" s="1">
+        <v>0</v>
+      </c>
+      <c r="D11" s="1">
+        <v>410</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="F11" s="1">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="15" t="s">
+        <v>296</v>
+      </c>
+      <c r="B12" s="1">
+        <v>2</v>
+      </c>
+      <c r="C12" s="1">
+        <v>0</v>
+      </c>
+      <c r="D12" s="1">
+        <v>300</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="F12" s="1">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="15" t="s">
+        <v>301</v>
+      </c>
+      <c r="B13" s="1">
+        <v>1</v>
+      </c>
+      <c r="C13" s="1">
+        <v>0</v>
+      </c>
+      <c r="D13" s="1">
+        <v>200</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="F13" s="1">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="15" t="s">
+        <v>297</v>
+      </c>
+      <c r="B14" s="1">
+        <v>1</v>
+      </c>
+      <c r="C14" s="1">
+        <v>0</v>
+      </c>
+      <c r="D14" s="1">
+        <v>160</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="F14" s="1">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="15" t="s">
+        <v>298</v>
+      </c>
+      <c r="B15" s="1">
+        <v>1</v>
+      </c>
+      <c r="C15" s="1">
+        <v>0</v>
+      </c>
+      <c r="D15" s="1">
+        <v>720</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="F15" s="1">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="15" t="s">
+        <v>300</v>
+      </c>
+      <c r="B16" s="1">
+        <v>0</v>
+      </c>
+      <c r="C16" s="1">
+        <v>0</v>
+      </c>
+      <c r="D16" s="1">
+        <v>0</v>
+      </c>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="15" t="s">
+        <v>299</v>
+      </c>
+      <c r="B17" s="1">
+        <v>1</v>
+      </c>
+      <c r="C17" s="1">
+        <v>0</v>
+      </c>
+      <c r="D17" s="1">
+        <v>190</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="F17" s="1">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{705C8F8E-56DC-45B6-9939-45B902DFD251}">
+  <dimension ref="A1:F17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="32.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>208</v>
+      </c>
+      <c r="B1" t="s">
+        <v>286</v>
+      </c>
+      <c r="C1" t="s">
+        <v>279</v>
+      </c>
+      <c r="D1" t="s">
+        <v>280</v>
+      </c>
+      <c r="E1" t="s">
+        <v>287</v>
+      </c>
+      <c r="F1" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>291</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1">
+        <v>6.91</v>
+      </c>
+      <c r="D2" s="1">
+        <v>-8.64</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="F2" s="1">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>292</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1">
+        <v>2.4</v>
+      </c>
+      <c r="D3" s="1">
+        <v>231</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="F3" s="1">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>294</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="10" t="s">
+        <v>290</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0</v>
+      </c>
+      <c r="D6" s="1">
+        <v>3.5</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>310</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1</v>
+      </c>
+      <c r="C7" s="1">
+        <v>39.753793103448274</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="F7" s="1">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>288</v>
+      </c>
+      <c r="B8" s="1">
+        <v>1</v>
+      </c>
+      <c r="C8" s="1">
+        <v>9.5</v>
+      </c>
+      <c r="D8" s="1">
+        <v>161.5</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="F8" s="1">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>289</v>
+      </c>
+      <c r="B9" s="1">
+        <v>1</v>
+      </c>
+      <c r="C9" s="1">
+        <v>3</v>
+      </c>
+      <c r="D9" s="1">
+        <v>51</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="F9" s="1">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>284</v>
+      </c>
+      <c r="B10" s="1">
+        <v>1</v>
+      </c>
+      <c r="C10" s="1">
+        <v>11.5</v>
+      </c>
+      <c r="D10" s="1">
+        <v>195.5</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="F10" s="1">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>295</v>
+      </c>
+      <c r="B11" s="1">
+        <v>0</v>
+      </c>
+      <c r="C11" s="1">
+        <v>0</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0</v>
+      </c>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>296</v>
+      </c>
+      <c r="B12" s="1">
+        <v>0</v>
+      </c>
+      <c r="C12" s="1">
+        <v>0</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0</v>
+      </c>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>301</v>
+      </c>
+      <c r="B13" s="1">
+        <v>0</v>
+      </c>
+      <c r="C13" s="1">
+        <v>0</v>
+      </c>
+      <c r="D13" s="1">
+        <v>0</v>
+      </c>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>297</v>
+      </c>
+      <c r="B14" s="1">
+        <v>0</v>
+      </c>
+      <c r="C14" s="1">
+        <v>0</v>
+      </c>
+      <c r="D14" s="1">
+        <v>0</v>
+      </c>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>298</v>
+      </c>
+      <c r="B15" s="1">
+        <v>0</v>
+      </c>
+      <c r="C15" s="1">
+        <v>0</v>
+      </c>
+      <c r="D15" s="1">
+        <v>0</v>
+      </c>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>300</v>
+      </c>
+      <c r="B16" s="1">
+        <v>1</v>
+      </c>
+      <c r="C16" s="1">
+        <v>0</v>
+      </c>
+      <c r="D16" s="1">
+        <v>200</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="F16" s="1">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>299</v>
+      </c>
+      <c r="B17" s="1">
+        <v>0</v>
+      </c>
+      <c r="C17" s="1">
+        <v>0</v>
+      </c>
+      <c r="D17" s="1">
+        <v>0</v>
+      </c>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A766E56F-5991-40E3-98F7-3876634381DF}">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -2113,7 +3673,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{790C9274-B2D0-4CB1-A413-BFF03ACE11B8}">
   <dimension ref="A1:D32"/>
   <sheetViews>
@@ -2537,7 +4097,7 @@
     </row>
     <row r="28" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="15" t="s">
-        <v>317</v>
+        <v>305</v>
       </c>
       <c r="B28" s="7">
         <f t="shared" si="1"/>
@@ -2615,7 +4175,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24394527-83C9-43E1-99B9-F6C50D02F0E0}">
   <dimension ref="A1:H91"/>
   <sheetViews>
@@ -5268,7 +6828,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FC79EF4-77A1-48AD-8822-597C66753CF5}">
   <dimension ref="A1:D22"/>
   <sheetViews>
@@ -5622,7 +7182,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{978F0E61-D55E-4846-92CF-DA7BB2817A97}">
   <dimension ref="A1:F4"/>
   <sheetViews>
@@ -5728,12 +7288,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC19E309-23D5-4D0A-B316-FCB0CC8B49A8}">
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5822,7 +7382,50 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10D61237-AECC-44ED-A2C5-2BB79F456807}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="20.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="15" t="s">
+        <v>208</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="9" t="s">
+        <v>227</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1.2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{689D00CC-D75A-4DA9-B2EA-0CA83BEECCA6}">
   <dimension ref="A1:G3"/>
   <sheetViews>
@@ -5917,7 +7520,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7FE94D6-2983-4058-A10D-F319D379B239}">
   <dimension ref="A1:G11"/>
   <sheetViews>
@@ -6210,7 +7813,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3B9F0F9-D24F-4187-97FF-36498970686A}">
   <dimension ref="A1:G14"/>
   <sheetViews>
@@ -6583,7 +8186,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A4F4307-4CCE-4E39-8D04-CE4F082A04BF}">
   <dimension ref="A1:D3"/>
   <sheetViews>
@@ -6640,50 +8243,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10D61237-AECC-44ED-A2C5-2BB79F456807}">
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="20.109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" s="15" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
-        <v>208</v>
-      </c>
-      <c r="B1" s="15" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="3">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="9" t="s">
-        <v>227</v>
-      </c>
-      <c r="B3" s="1">
-        <v>1.2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC1C16C4-514C-4855-AC00-5CBAF6F7CA67}">
   <dimension ref="A1:L62"/>
   <sheetViews>
@@ -8877,15 +10437,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44ACC5D0-181B-4F4E-94F7-26883B6AC5A8}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A7"/>
+      <selection activeCell="A2" sqref="A2:A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.44140625" style="9" customWidth="1"/>
   </cols>
   <sheetData>
@@ -8899,7 +10459,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>278</v>
+        <v>312</v>
       </c>
       <c r="B2" s="1">
         <v>0.9</v>
@@ -8907,7 +10467,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>279</v>
+        <v>313</v>
       </c>
       <c r="B3" s="1">
         <v>0.3</v>
@@ -8915,29 +10475,11 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>280</v>
+        <v>314</v>
       </c>
       <c r="B4" s="1">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="9" t="s">
-        <v>284</v>
-      </c>
-      <c r="B5" s="1"/>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="9" t="s">
-        <v>285</v>
-      </c>
-      <c r="B6" s="1"/>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="9" t="s">
-        <v>286</v>
-      </c>
-      <c r="B7" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8946,11 +10488,90 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CF77810-B06B-4FCF-A7A9-1A41CBB598D4}">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="23.109375" style="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.44140625" style="15" customWidth="1"/>
+    <col min="3" max="16384" width="8.88671875" style="15"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="15" t="s">
+        <v>208</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="15" t="s">
+        <v>312</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="15" t="s">
+        <v>313</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="15" t="s">
+        <v>314</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="15" t="s">
+        <v>315</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="15" t="s">
+        <v>316</v>
+      </c>
+      <c r="B6" s="13">
+        <f>55/45*B5</f>
+        <v>0.73333333333333339</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="15" t="s">
+        <v>317</v>
+      </c>
+      <c r="B7" s="13">
+        <f>45/55*B5</f>
+        <v>0.49090909090909091</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07987B69-2230-4E5F-926C-42312732B1EC}">
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="A2" sqref="A2:A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8968,7 +10589,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
-        <v>281</v>
+        <v>312</v>
       </c>
       <c r="B2" s="1">
         <v>0.4</v>
@@ -8976,7 +10597,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
-        <v>282</v>
+        <v>313</v>
       </c>
       <c r="B3" s="1">
         <v>0.2</v>
@@ -8984,7 +10605,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
-        <v>283</v>
+        <v>314</v>
       </c>
       <c r="B4" s="1">
         <v>1.5</v>
@@ -8992,7 +10613,7 @@
     </row>
     <row r="5" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
-        <v>290</v>
+        <v>315</v>
       </c>
       <c r="B5" s="1">
         <v>0.2</v>
@@ -9000,7 +10621,7 @@
     </row>
     <row r="6" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
-        <v>287</v>
+        <v>316</v>
       </c>
       <c r="B6" s="13">
         <f>55/45*B5</f>
@@ -9009,7 +10630,7 @@
     </row>
     <row r="7" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
-        <v>288</v>
+        <v>317</v>
       </c>
       <c r="B7" s="13">
         <f>45/55*B5</f>
@@ -9022,13 +10643,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D89349C-4881-488D-B8C5-0F08759EC631}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -9081,7 +10700,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>289</v>
+        <v>278</v>
       </c>
       <c r="B3" s="1">
         <v>8.4699999999999997E-8</v>
@@ -9106,12 +10725,163 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D16EAC8-38E2-4645-A6B8-8BBE98EEE76B}">
-  <dimension ref="A1:F5"/>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{296F017F-5D07-49B3-8EFA-D60107F0927C}">
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="A16" sqref="A16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="28.44140625" style="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.88671875" style="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.44140625" style="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="12" style="15" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.6640625" style="15" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.88671875" style="15"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="15" t="s">
+        <v>208</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>271</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>272</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>273</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>274</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="15" t="s">
+        <v>306</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1">
+        <v>0</v>
+      </c>
+      <c r="D2" s="1">
+        <f>4*0.001</f>
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="E2" s="1">
+        <f>25*0.141</f>
+        <v>3.5249999999999995</v>
+      </c>
+      <c r="F2" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="15" t="s">
+        <v>307</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1">
+        <v>2.7900000000000001E-2</v>
+      </c>
+      <c r="E3" s="1">
+        <v>-13.269</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="15" t="s">
+        <v>275</v>
+      </c>
+      <c r="B4" s="1">
+        <v>-9.556E-5</v>
+      </c>
+      <c r="C4" s="1">
+        <v>2.652171E-2</v>
+      </c>
+      <c r="D4" s="1">
+        <v>-2.5608517599999998</v>
+      </c>
+      <c r="E4" s="1">
+        <v>193.19055123999999</v>
+      </c>
+      <c r="F4" s="1">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="15" t="s">
+        <v>278</v>
+      </c>
+      <c r="B5" s="1">
+        <v>8.4699999999999997E-8</v>
+      </c>
+      <c r="C5" s="1">
+        <v>-2.4901100000000001E-5</v>
+      </c>
+      <c r="D5" s="1">
+        <v>2.3686407999999998E-3</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0.1245668155</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F15" s="17"/>
+      <c r="G15" s="17"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F16" s="17"/>
+      <c r="G16" s="17"/>
+    </row>
+    <row r="17" spans="6:7" x14ac:dyDescent="0.3">
+      <c r="F17" s="17"/>
+      <c r="G17" s="17"/>
+    </row>
+    <row r="18" spans="6:7" x14ac:dyDescent="0.3">
+      <c r="F18" s="17"/>
+      <c r="G18" s="17"/>
+    </row>
+    <row r="19" spans="6:7" x14ac:dyDescent="0.3">
+      <c r="F19" s="17"/>
+      <c r="G19" s="17"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D16EAC8-38E2-4645-A6B8-8BBE98EEE76B}">
+  <dimension ref="A1:G19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14:G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9125,7 +10895,7 @@
     <col min="7" max="7" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="15" t="s">
         <v>208</v>
       </c>
@@ -9145,9 +10915,9 @@
         <v>217</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
-        <v>318</v>
+        <v>306</v>
       </c>
       <c r="B2" s="1">
         <v>0</v>
@@ -9165,9 +10935,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
-        <v>319</v>
+        <v>307</v>
       </c>
       <c r="B3" s="1">
         <v>0</v>
@@ -9185,9 +10955,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="15" t="s">
-        <v>289</v>
+        <v>278</v>
       </c>
       <c r="B4" s="1">
         <v>0</v>
@@ -9205,7 +10975,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="15" t="s">
         <v>275</v>
       </c>
@@ -9224,6 +10994,35 @@
       <c r="F5" s="1">
         <v>2017</v>
       </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E15" s="15"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="17"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E16" s="15"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="17"/>
+    </row>
+    <row r="17" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E17" s="15"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="17"/>
+    </row>
+    <row r="18" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E18" s="15"/>
+      <c r="F18" s="17"/>
+      <c r="G18" s="17"/>
+    </row>
+    <row r="19" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E19" s="15"/>
+      <c r="F19" s="17"/>
+      <c r="G19" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9231,7 +11030,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D1A1908-ADF0-4823-836D-799AF3E6FC99}">
   <dimension ref="A1:F17"/>
   <sheetViews>
@@ -9253,16 +11052,16 @@
         <v>208</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>298</v>
+        <v>286</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>291</v>
+        <v>279</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>292</v>
+        <v>280</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>299</v>
+        <v>287</v>
       </c>
       <c r="F1" s="15" t="s">
         <v>217</v>
@@ -9270,7 +11069,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
-        <v>303</v>
+        <v>291</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
@@ -9282,7 +11081,7 @@
         <v>0</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>314</v>
+        <v>302</v>
       </c>
       <c r="F2" s="1">
         <v>2019</v>
@@ -9290,7 +11089,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="15" t="s">
-        <v>304</v>
+        <v>292</v>
       </c>
       <c r="B3" s="1">
         <v>1</v>
@@ -9302,7 +11101,7 @@
         <v>0</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>314</v>
+        <v>302</v>
       </c>
       <c r="F3" s="1">
         <v>2019</v>
@@ -9310,7 +11109,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="15" t="s">
-        <v>305</v>
+        <v>293</v>
       </c>
       <c r="B4" s="1">
         <v>0</v>
@@ -9328,7 +11127,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="15" t="s">
-        <v>306</v>
+        <v>294</v>
       </c>
       <c r="B5" s="1">
         <v>0</v>
@@ -9346,7 +11145,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
-        <v>302</v>
+        <v>290</v>
       </c>
       <c r="B6" s="1">
         <v>1</v>
@@ -9358,7 +11157,7 @@
         <v>3.5</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>321</v>
+        <v>309</v>
       </c>
       <c r="F6" s="1">
         <v>0</v>
@@ -9366,7 +11165,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="15" t="s">
-        <v>322</v>
+        <v>310</v>
       </c>
       <c r="B7" s="1">
         <v>1</v>
@@ -9378,7 +11177,7 @@
         <v>0</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>315</v>
+        <v>303</v>
       </c>
       <c r="F7" s="1">
         <v>2019</v>
@@ -9386,7 +11185,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="15" t="s">
-        <v>300</v>
+        <v>288</v>
       </c>
       <c r="B8" s="1">
         <v>1</v>
@@ -9398,7 +11197,7 @@
         <v>161.5</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>295</v>
+        <v>283</v>
       </c>
       <c r="F8" s="1">
         <v>2019</v>
@@ -9406,7 +11205,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="15" t="s">
-        <v>301</v>
+        <v>289</v>
       </c>
       <c r="B9" s="1">
         <v>1</v>
@@ -9418,7 +11217,7 @@
         <v>51</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>295</v>
+        <v>283</v>
       </c>
       <c r="F9" s="1">
         <v>2019</v>
@@ -9426,7 +11225,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="15" t="s">
-        <v>296</v>
+        <v>284</v>
       </c>
       <c r="B10" s="1">
         <v>1</v>
@@ -9438,7 +11237,7 @@
         <v>195.5</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>295</v>
+        <v>283</v>
       </c>
       <c r="F10" s="1">
         <v>2019</v>
@@ -9446,7 +11245,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="15" t="s">
-        <v>307</v>
+        <v>295</v>
       </c>
       <c r="B11" s="1">
         <v>1</v>
@@ -9458,7 +11257,7 @@
         <v>410</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>297</v>
+        <v>285</v>
       </c>
       <c r="F11" s="1">
         <v>2019</v>
@@ -9466,7 +11265,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="15" t="s">
-        <v>308</v>
+        <v>296</v>
       </c>
       <c r="B12" s="1">
         <v>1</v>
@@ -9478,7 +11277,7 @@
         <v>300</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>297</v>
+        <v>285</v>
       </c>
       <c r="F12" s="1">
         <v>2019</v>
@@ -9486,7 +11285,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="15" t="s">
-        <v>313</v>
+        <v>301</v>
       </c>
       <c r="B13" s="1">
         <v>1</v>
@@ -9498,7 +11297,7 @@
         <v>200</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>297</v>
+        <v>285</v>
       </c>
       <c r="F13" s="1">
         <v>2019</v>
@@ -9506,7 +11305,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="15" t="s">
-        <v>309</v>
+        <v>297</v>
       </c>
       <c r="B14" s="1">
         <v>1</v>
@@ -9518,7 +11317,7 @@
         <v>160</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>297</v>
+        <v>285</v>
       </c>
       <c r="F14" s="1">
         <v>2019</v>
@@ -9526,7 +11325,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="15" t="s">
-        <v>310</v>
+        <v>298</v>
       </c>
       <c r="B15" s="1">
         <v>1</v>
@@ -9538,7 +11337,7 @@
         <v>720</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>297</v>
+        <v>285</v>
       </c>
       <c r="F15" s="1">
         <v>2019</v>
@@ -9546,7 +11345,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="15" t="s">
-        <v>312</v>
+        <v>300</v>
       </c>
       <c r="B16" s="1">
         <v>0</v>
@@ -9564,7 +11363,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="15" t="s">
-        <v>311</v>
+        <v>299</v>
       </c>
       <c r="B17" s="1">
         <v>0</v>
@@ -9585,710 +11384,4 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4932C69-09AA-44A9-AC5E-22F05F727E1B}">
-  <dimension ref="A1:F17"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="32.6640625" style="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="8.88671875" style="15"/>
-    <col min="5" max="5" width="33.21875" style="15" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.6640625" style="15" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.88671875" style="15"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
-        <v>208</v>
-      </c>
-      <c r="B1" s="15" t="s">
-        <v>298</v>
-      </c>
-      <c r="C1" s="15" t="s">
-        <v>291</v>
-      </c>
-      <c r="D1" s="15" t="s">
-        <v>292</v>
-      </c>
-      <c r="E1" s="15" t="s">
-        <v>299</v>
-      </c>
-      <c r="F1" s="15" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="15" t="s">
-        <v>303</v>
-      </c>
-      <c r="B2" s="1">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1">
-        <v>4.29</v>
-      </c>
-      <c r="D2" s="1">
-        <v>0</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>316</v>
-      </c>
-      <c r="F2" s="1">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="15" t="s">
-        <v>304</v>
-      </c>
-      <c r="B3" s="1">
-        <v>1</v>
-      </c>
-      <c r="C3" s="1">
-        <v>2.5</v>
-      </c>
-      <c r="D3" s="1">
-        <v>0</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>316</v>
-      </c>
-      <c r="F3" s="1">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="15" t="s">
-        <v>305</v>
-      </c>
-      <c r="B4" s="1">
-        <v>1</v>
-      </c>
-      <c r="C4" s="1">
-        <v>3.12</v>
-      </c>
-      <c r="D4" s="1">
-        <v>0</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>316</v>
-      </c>
-      <c r="F4" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="15" t="s">
-        <v>306</v>
-      </c>
-      <c r="B5" s="1">
-        <v>1</v>
-      </c>
-      <c r="C5" s="1">
-        <v>4</v>
-      </c>
-      <c r="D5" s="1">
-        <v>0</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>316</v>
-      </c>
-      <c r="F5" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="10" t="s">
-        <v>302</v>
-      </c>
-      <c r="B6" s="1">
-        <v>1</v>
-      </c>
-      <c r="C6" s="1">
-        <v>0</v>
-      </c>
-      <c r="D6" s="1">
-        <v>3.5</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>321</v>
-      </c>
-      <c r="F6" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="15" t="s">
-        <v>322</v>
-      </c>
-      <c r="B7" s="1">
-        <v>1</v>
-      </c>
-      <c r="C7" s="1">
-        <v>39.753793103448274</v>
-      </c>
-      <c r="D7" s="1">
-        <v>0</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>315</v>
-      </c>
-      <c r="F7" s="1">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="15" t="s">
-        <v>300</v>
-      </c>
-      <c r="B8" s="1">
-        <v>1</v>
-      </c>
-      <c r="C8" s="1">
-        <v>9.5</v>
-      </c>
-      <c r="D8" s="1">
-        <v>161.5</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>295</v>
-      </c>
-      <c r="F8" s="1">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="15" t="s">
-        <v>301</v>
-      </c>
-      <c r="B9" s="1">
-        <v>1</v>
-      </c>
-      <c r="C9" s="1">
-        <v>3</v>
-      </c>
-      <c r="D9" s="1">
-        <v>51</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>295</v>
-      </c>
-      <c r="F9" s="1">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="15" t="s">
-        <v>296</v>
-      </c>
-      <c r="B10" s="1">
-        <v>1</v>
-      </c>
-      <c r="C10" s="1">
-        <v>11.5</v>
-      </c>
-      <c r="D10" s="1">
-        <v>195.5</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>295</v>
-      </c>
-      <c r="F10" s="1">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="15" t="s">
-        <v>307</v>
-      </c>
-      <c r="B11" s="1">
-        <v>2</v>
-      </c>
-      <c r="C11" s="1">
-        <v>0</v>
-      </c>
-      <c r="D11" s="1">
-        <v>410</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>297</v>
-      </c>
-      <c r="F11" s="1">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="15" t="s">
-        <v>308</v>
-      </c>
-      <c r="B12" s="1">
-        <v>2</v>
-      </c>
-      <c r="C12" s="1">
-        <v>0</v>
-      </c>
-      <c r="D12" s="1">
-        <v>300</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>297</v>
-      </c>
-      <c r="F12" s="1">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="15" t="s">
-        <v>313</v>
-      </c>
-      <c r="B13" s="1">
-        <v>1</v>
-      </c>
-      <c r="C13" s="1">
-        <v>0</v>
-      </c>
-      <c r="D13" s="1">
-        <v>200</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>297</v>
-      </c>
-      <c r="F13" s="1">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="15" t="s">
-        <v>309</v>
-      </c>
-      <c r="B14" s="1">
-        <v>1</v>
-      </c>
-      <c r="C14" s="1">
-        <v>0</v>
-      </c>
-      <c r="D14" s="1">
-        <v>160</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>297</v>
-      </c>
-      <c r="F14" s="1">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="15" t="s">
-        <v>310</v>
-      </c>
-      <c r="B15" s="1">
-        <v>1</v>
-      </c>
-      <c r="C15" s="1">
-        <v>0</v>
-      </c>
-      <c r="D15" s="1">
-        <v>720</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>297</v>
-      </c>
-      <c r="F15" s="1">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="15" t="s">
-        <v>312</v>
-      </c>
-      <c r="B16" s="1">
-        <v>0</v>
-      </c>
-      <c r="C16" s="1">
-        <v>0</v>
-      </c>
-      <c r="D16" s="1">
-        <v>0</v>
-      </c>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="15" t="s">
-        <v>311</v>
-      </c>
-      <c r="B17" s="1">
-        <v>1</v>
-      </c>
-      <c r="C17" s="1">
-        <v>0</v>
-      </c>
-      <c r="D17" s="1">
-        <v>190</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>297</v>
-      </c>
-      <c r="F17" s="1">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{705C8F8E-56DC-45B6-9939-45B902DFD251}">
-  <dimension ref="A1:F17"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="32.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="33.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>208</v>
-      </c>
-      <c r="B1" t="s">
-        <v>298</v>
-      </c>
-      <c r="C1" t="s">
-        <v>291</v>
-      </c>
-      <c r="D1" t="s">
-        <v>292</v>
-      </c>
-      <c r="E1" t="s">
-        <v>299</v>
-      </c>
-      <c r="F1" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>303</v>
-      </c>
-      <c r="B2" s="1">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1">
-        <v>6.91</v>
-      </c>
-      <c r="D2" s="1">
-        <v>-8.64</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="F2" s="1">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>304</v>
-      </c>
-      <c r="B3" s="1">
-        <v>1</v>
-      </c>
-      <c r="C3" s="1">
-        <v>2.4</v>
-      </c>
-      <c r="D3" s="1">
-        <v>231</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="F3" s="1">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>305</v>
-      </c>
-      <c r="B4" s="1">
-        <v>0</v>
-      </c>
-      <c r="C4" s="1">
-        <v>0</v>
-      </c>
-      <c r="D4" s="1">
-        <v>0</v>
-      </c>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>306</v>
-      </c>
-      <c r="B5" s="1">
-        <v>0</v>
-      </c>
-      <c r="C5" s="1">
-        <v>0</v>
-      </c>
-      <c r="D5" s="1">
-        <v>0</v>
-      </c>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="10" t="s">
-        <v>302</v>
-      </c>
-      <c r="B6" s="1">
-        <v>1</v>
-      </c>
-      <c r="C6" s="1">
-        <v>0</v>
-      </c>
-      <c r="D6" s="1">
-        <v>3.5</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>323</v>
-      </c>
-      <c r="F6" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>322</v>
-      </c>
-      <c r="B7" s="1">
-        <v>1</v>
-      </c>
-      <c r="C7" s="1">
-        <v>39.753793103448274</v>
-      </c>
-      <c r="D7" s="1">
-        <v>0</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>294</v>
-      </c>
-      <c r="F7" s="1">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>300</v>
-      </c>
-      <c r="B8" s="1">
-        <v>1</v>
-      </c>
-      <c r="C8" s="1">
-        <v>9.5</v>
-      </c>
-      <c r="D8" s="1">
-        <v>161.5</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>295</v>
-      </c>
-      <c r="F8" s="1">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>301</v>
-      </c>
-      <c r="B9" s="1">
-        <v>1</v>
-      </c>
-      <c r="C9" s="1">
-        <v>3</v>
-      </c>
-      <c r="D9" s="1">
-        <v>51</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>295</v>
-      </c>
-      <c r="F9" s="1">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>296</v>
-      </c>
-      <c r="B10" s="1">
-        <v>1</v>
-      </c>
-      <c r="C10" s="1">
-        <v>11.5</v>
-      </c>
-      <c r="D10" s="1">
-        <v>195.5</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>295</v>
-      </c>
-      <c r="F10" s="1">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>307</v>
-      </c>
-      <c r="B11" s="1">
-        <v>0</v>
-      </c>
-      <c r="C11" s="1">
-        <v>0</v>
-      </c>
-      <c r="D11" s="1">
-        <v>0</v>
-      </c>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>308</v>
-      </c>
-      <c r="B12" s="1">
-        <v>0</v>
-      </c>
-      <c r="C12" s="1">
-        <v>0</v>
-      </c>
-      <c r="D12" s="1">
-        <v>0</v>
-      </c>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>313</v>
-      </c>
-      <c r="B13" s="1">
-        <v>0</v>
-      </c>
-      <c r="C13" s="1">
-        <v>0</v>
-      </c>
-      <c r="D13" s="1">
-        <v>0</v>
-      </c>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>309</v>
-      </c>
-      <c r="B14" s="1">
-        <v>0</v>
-      </c>
-      <c r="C14" s="1">
-        <v>0</v>
-      </c>
-      <c r="D14" s="1">
-        <v>0</v>
-      </c>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>310</v>
-      </c>
-      <c r="B15" s="1">
-        <v>0</v>
-      </c>
-      <c r="C15" s="1">
-        <v>0</v>
-      </c>
-      <c r="D15" s="1">
-        <v>0</v>
-      </c>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>312</v>
-      </c>
-      <c r="B16" s="1">
-        <v>1</v>
-      </c>
-      <c r="C16" s="1">
-        <v>0</v>
-      </c>
-      <c r="D16" s="1">
-        <v>200</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>297</v>
-      </c>
-      <c r="F16" s="1">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>311</v>
-      </c>
-      <c r="B17" s="1">
-        <v>0</v>
-      </c>
-      <c r="C17" s="1">
-        <v>0</v>
-      </c>
-      <c r="D17" s="1">
-        <v>0</v>
-      </c>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Add Aftertreatment class as a start to calculating CAP-related costs. Add aftertreatment cost metrics to alpha_package_costs_module_inputs.xlsx.
</commit_message>
<xml_diff>
--- a/omega_preproc/alpha_package_costs/inputs/alpha_package_costs_module_inputs.xlsx
+++ b/omega_preproc/alpha_package_costs/inputs/alpha_package_costs_module_inputs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TSHERWOO\PycharmProjects\EPA_OMEGA_Model\omega_preproc\alpha_package_costs\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2C070C6-9D15-454C-8D32-B53292941B56}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9831754F-00AE-4368-939F-EC1A22822053}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="960" yWindow="960" windowWidth="21600" windowHeight="11205" tabRatio="826" xr2:uid="{31AE0ECC-ADD6-46A3-9F50-4BA6582DDF8B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="826" firstSheet="8" activeTab="21" xr2:uid="{31AE0ECC-ADD6-46A3-9F50-4BA6582DDF8B}"/>
   </bookViews>
   <sheets>
     <sheet name="inputs_code" sheetId="15" r:id="rId1"/>
@@ -34,7 +34,8 @@
     <sheet name="aero" sheetId="6" r:id="rId19"/>
     <sheet name="nonaero" sheetId="9" r:id="rId20"/>
     <sheet name="ac" sheetId="17" r:id="rId21"/>
-    <sheet name="et_dmc" sheetId="7" r:id="rId22"/>
+    <sheet name="aftertreatment" sheetId="33" r:id="rId22"/>
+    <sheet name="et_dmc" sheetId="7" r:id="rId23"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="18" hidden="1">aero!$B$1:$E$3</definedName>
@@ -457,7 +458,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1028" uniqueCount="323">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1061" uniqueCount="350">
   <si>
     <t>Markup</t>
   </si>
@@ -1426,6 +1427,87 @@
   </si>
   <si>
     <t>DC-DC kW (3.5) + OBC kW (0.7,1.1,1.9)</t>
+  </si>
+  <si>
+    <t>dmc_slope</t>
+  </si>
+  <si>
+    <t>dmc_intercept</t>
+  </si>
+  <si>
+    <t>http://www.platinum.matthey.com/prices/price-tables</t>
+  </si>
+  <si>
+    <t>Month Average for all time zones (20220125)</t>
+  </si>
+  <si>
+    <t>ibid</t>
+  </si>
+  <si>
+    <t>SAE 2013-01-0534</t>
+  </si>
+  <si>
+    <t>Tier3</t>
+  </si>
+  <si>
+    <t>substrate_twc</t>
+  </si>
+  <si>
+    <t>washcoat_twc</t>
+  </si>
+  <si>
+    <t>canning_twc</t>
+  </si>
+  <si>
+    <t>swept_volume_twc</t>
+  </si>
+  <si>
+    <t>substrate_gpf</t>
+  </si>
+  <si>
+    <t>washcoat_gpf</t>
+  </si>
+  <si>
+    <t>canning_gpf</t>
+  </si>
+  <si>
+    <t>swept_volume_gpf</t>
+  </si>
+  <si>
+    <t>Pt_dollars_per_troy_oz</t>
+  </si>
+  <si>
+    <t>Pd_dollars_per_troy_oz</t>
+  </si>
+  <si>
+    <t>Rh_dollars_per_troy_oz</t>
+  </si>
+  <si>
+    <t>Pt_grams_per_liter_twc</t>
+  </si>
+  <si>
+    <t>Pd_grams_per_liter_twc</t>
+  </si>
+  <si>
+    <t>Rh_grams_per_liter_twc</t>
+  </si>
+  <si>
+    <t>markup_twc</t>
+  </si>
+  <si>
+    <t>markup_gpf</t>
+  </si>
+  <si>
+    <t>learning_rate_aftertreatment</t>
+  </si>
+  <si>
+    <t>Pt_grams_per_liter_gpf</t>
+  </si>
+  <si>
+    <t>Pd_grams_per_liter_gpf</t>
+  </si>
+  <si>
+    <t>Rh_grams_per_liter_gpf</t>
   </si>
 </sst>
 </file>
@@ -1438,7 +1520,7 @@
     <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1580,8 +1662,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF9C6500"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1601,6 +1695,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
   </fills>
@@ -1652,7 +1751,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="35">
+  <cellStyleXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
@@ -1688,8 +1787,12 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="16" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="22" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1714,13 +1817,16 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="4" fillId="2" borderId="1" xfId="5" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="1" xfId="5" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="35">
+  <cellStyles count="39">
     <cellStyle name="Accent1 2" xfId="20" xr:uid="{D9FD632B-EF7F-49B6-8440-0774D2DADADB}"/>
     <cellStyle name="Calculation" xfId="31" builtinId="22"/>
     <cellStyle name="Calculation 2" xfId="14" xr:uid="{FE108587-6BB1-48C6-A201-65192C808774}"/>
     <cellStyle name="Calculation 2 2" xfId="33" xr:uid="{271F3B4E-206F-401C-B81A-8EA46F45418D}"/>
     <cellStyle name="Calculation 3" xfId="6" xr:uid="{5274EEA8-4A6C-49CF-911D-0B513965EDE0}"/>
+    <cellStyle name="Calculation 3 2" xfId="35" xr:uid="{BA602260-5A7A-4EDF-A2B0-B5C5B6E1B801}"/>
     <cellStyle name="Calculation 4" xfId="24" xr:uid="{E581566A-4310-498D-B20D-DE28C46FA6DF}"/>
     <cellStyle name="Comma 2" xfId="16" xr:uid="{6C404ECA-4D34-4FDB-9417-7D5B37CECF6C}"/>
     <cellStyle name="Comma 3" xfId="15" xr:uid="{2C18F2F8-CABC-4993-A5E7-40DF4A6C346C}"/>
@@ -1733,6 +1839,7 @@
     <cellStyle name="Linked Cell 2" xfId="17" xr:uid="{E76B1D5C-B61E-4A12-A6A9-914B9635274E}"/>
     <cellStyle name="Linked Cell 2 2" xfId="34" xr:uid="{9CDC69F0-4BDB-4E6B-96DF-9997EAD764BB}"/>
     <cellStyle name="Linked Cell 3" xfId="7" xr:uid="{A4E24AE6-00B3-41A9-BD71-207B6B1CFE7F}"/>
+    <cellStyle name="Neutral 2" xfId="38" xr:uid="{DA0D5CE0-0206-438D-878A-329806984A81}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{BB3C9F31-2AF0-4A34-BF88-C635292282C0}"/>
     <cellStyle name="Normal 2 2" xfId="28" xr:uid="{619E91A8-96B2-4336-A945-E172440606C8}"/>
@@ -1745,12 +1852,14 @@
     <cellStyle name="Normal 5" xfId="8" xr:uid="{67E3CCE3-ADF3-4EA9-9DD7-5499299E58B1}"/>
     <cellStyle name="Normal 6" xfId="21" xr:uid="{E30054B3-EB6B-45E1-B681-D9CAAB0ABBFF}"/>
     <cellStyle name="Normal 7" xfId="3" xr:uid="{C6E5CA8E-5BF8-4D04-B0E4-0F911B37164F}"/>
+    <cellStyle name="Normal 7 2" xfId="36" xr:uid="{DBA63DBB-099B-4F0E-9C67-34B6351D8774}"/>
     <cellStyle name="Output" xfId="23" builtinId="21"/>
     <cellStyle name="Output 2" xfId="19" xr:uid="{E4B9B678-BB91-49BE-9466-2B18699E335C}"/>
     <cellStyle name="Percent 2" xfId="9" xr:uid="{853BFCA4-8A84-4DA7-A80C-99F2129715B2}"/>
     <cellStyle name="Percent 2 2" xfId="26" xr:uid="{980F5F3C-CB52-4C6B-9481-5B24D30F92F3}"/>
     <cellStyle name="Percent 3" xfId="10" xr:uid="{1573D7D6-7F3E-4DB1-9CC8-18AD53222C70}"/>
     <cellStyle name="Percent 4" xfId="4" xr:uid="{E1B2A24A-4C5A-4471-AE28-D80443CC02B4}"/>
+    <cellStyle name="Percent 4 2" xfId="37" xr:uid="{54DE988F-4134-4D0C-8BD9-AB20B2F287B9}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2092,10 +2201,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF58B9CD-C45C-4464-97D6-845ECC18E560}">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2104,7 +2213,7 @@
     <col min="2" max="2" width="19.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>208</v>
       </c>
@@ -2112,7 +2221,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>276</v>
       </c>
@@ -2120,13 +2229,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>277</v>
       </c>
       <c r="B3" s="1"/>
     </row>
-    <row r="4" spans="1:2" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
         <v>308</v>
       </c>
@@ -2134,7 +2243,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="5" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>210</v>
       </c>
@@ -2142,7 +2251,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="6" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>211</v>
       </c>
@@ -2150,7 +2259,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>212</v>
       </c>
@@ -2158,7 +2267,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>263</v>
       </c>
@@ -2166,7 +2275,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>213</v>
       </c>
@@ -2174,7 +2283,7 @@
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>207</v>
       </c>
@@ -2182,7 +2291,7 @@
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:2" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
         <v>317</v>
       </c>
@@ -2190,11 +2299,55 @@
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
+    <row r="12" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>346</v>
+      </c>
+      <c r="B12" s="1">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="15" t="s">
+        <v>338</v>
+      </c>
+      <c r="B13" s="1">
+        <v>990.58</v>
+      </c>
+      <c r="C13" t="s">
+        <v>325</v>
+      </c>
+      <c r="D13" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="15" t="s">
+        <v>339</v>
+      </c>
+      <c r="B14" s="1">
+        <v>1952.23</v>
+      </c>
+      <c r="C14" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="15" t="s">
+        <v>340</v>
+      </c>
+      <c r="B15" s="1">
+        <v>16328.67</v>
+      </c>
+      <c r="C15" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B16" s="1">
         <v>1.2</v>
       </c>
     </row>
@@ -7537,6 +7690,262 @@
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2A32868-5770-4D9F-98C2-1E495D488F86}">
+  <dimension ref="A1:F17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14:A16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>208</v>
+      </c>
+      <c r="B1" t="s">
+        <v>209</v>
+      </c>
+      <c r="C1" t="s">
+        <v>323</v>
+      </c>
+      <c r="D1" t="s">
+        <v>324</v>
+      </c>
+      <c r="E1" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>330</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1">
+        <v>6.1080000000000005</v>
+      </c>
+      <c r="D2" s="1">
+        <v>1.9545599999999999</v>
+      </c>
+      <c r="E2" s="1">
+        <v>2012</v>
+      </c>
+      <c r="F2" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>331</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1">
+        <v>5.09</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1">
+        <v>2012</v>
+      </c>
+      <c r="F3" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>332</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1">
+        <v>2.4432</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1">
+        <v>2012</v>
+      </c>
+      <c r="F4" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>333</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1.2</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0</v>
+      </c>
+      <c r="F5" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>341</v>
+      </c>
+      <c r="B6" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="15" t="s">
+        <v>342</v>
+      </c>
+      <c r="B7" s="19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="15" t="s">
+        <v>343</v>
+      </c>
+      <c r="B8" s="19">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="15" t="s">
+        <v>344</v>
+      </c>
+      <c r="B9" s="18">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>334</v>
+      </c>
+      <c r="B10" s="1">
+        <v>0</v>
+      </c>
+      <c r="C10" s="1">
+        <v>1</v>
+      </c>
+      <c r="D10" s="1">
+        <v>1</v>
+      </c>
+      <c r="E10" s="1">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>335</v>
+      </c>
+      <c r="B11" s="1">
+        <v>0</v>
+      </c>
+      <c r="C11" s="1">
+        <v>1</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0</v>
+      </c>
+      <c r="E11" s="1">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>336</v>
+      </c>
+      <c r="B12" s="1">
+        <v>0</v>
+      </c>
+      <c r="C12" s="1">
+        <v>1</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0</v>
+      </c>
+      <c r="E12" s="1">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>337</v>
+      </c>
+      <c r="B13" s="1">
+        <v>1.2</v>
+      </c>
+      <c r="C13" s="1">
+        <v>0</v>
+      </c>
+      <c r="D13" s="1">
+        <v>0</v>
+      </c>
+      <c r="E13" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>347</v>
+      </c>
+      <c r="B14" s="19">
+        <v>1</v>
+      </c>
+      <c r="C14" s="15"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>348</v>
+      </c>
+      <c r="B15" s="19">
+        <v>0</v>
+      </c>
+      <c r="C15" s="15"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>349</v>
+      </c>
+      <c r="B16" s="19">
+        <v>0</v>
+      </c>
+      <c r="C16" s="15"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="15"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="15" t="s">
+        <v>345</v>
+      </c>
+      <c r="B17" s="18">
+        <v>1.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC1C16C4-514C-4855-AC00-5CBAF6F7CA67}">
   <dimension ref="A1:L62"/>
   <sheetViews>

</xml_diff>

<commit_message>
Update documentation with new aftertreatment costs.
</commit_message>
<xml_diff>
--- a/omega_preproc/alpha_package_costs/inputs/alpha_package_costs_module_inputs.xlsx
+++ b/omega_preproc/alpha_package_costs/inputs/alpha_package_costs_module_inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TSHERWOO\PycharmProjects\EPA_OMEGA_Model\omega_preproc\alpha_package_costs\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9831754F-00AE-4368-939F-EC1A22822053}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F6DFB47-F1BA-423A-8F29-0D7A71081478}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="826" firstSheet="8" activeTab="21" xr2:uid="{31AE0ECC-ADD6-46A3-9F50-4BA6582DDF8B}"/>
   </bookViews>
@@ -2204,7 +2204,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7694,7 +7694,7 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:A16"/>
+      <selection sqref="A1:E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Revise learning calcs in alpha_package_costs.py. Add new inputs to alpha_package_costs_module_inputs.xlsx.
</commit_message>
<xml_diff>
--- a/omega_preproc/alpha_package_costs/inputs/alpha_package_costs_module_inputs.xlsx
+++ b/omega_preproc/alpha_package_costs/inputs/alpha_package_costs_module_inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TSHERWOO\PycharmProjects\EPA_OMEGA_Model\omega_preproc\alpha_package_costs\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F6DFB47-F1BA-423A-8F29-0D7A71081478}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0AAB228-2CD3-48F9-8C6E-FF5CDF2B7A1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="826" firstSheet="8" activeTab="21" xr2:uid="{31AE0ECC-ADD6-46A3-9F50-4BA6582DDF8B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="826" xr2:uid="{31AE0ECC-ADD6-46A3-9F50-4BA6582DDF8B}"/>
   </bookViews>
   <sheets>
     <sheet name="inputs_code" sheetId="15" r:id="rId1"/>
@@ -458,7 +458,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1061" uniqueCount="350">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1071" uniqueCount="360">
   <si>
     <t>Markup</t>
   </si>
@@ -1508,6 +1508,36 @@
   </si>
   <si>
     <t>Rh_grams_per_liter_gpf</t>
+  </si>
+  <si>
+    <t>learning_rate</t>
+  </si>
+  <si>
+    <t>weight_sales_scaler</t>
+  </si>
+  <si>
+    <t>weight_scaler</t>
+  </si>
+  <si>
+    <t>ice_scaler</t>
+  </si>
+  <si>
+    <t>roadload_scaler</t>
+  </si>
+  <si>
+    <t>pev_scaler</t>
+  </si>
+  <si>
+    <t>roadload_sales_scaler</t>
+  </si>
+  <si>
+    <t>ice_sales_scaler</t>
+  </si>
+  <si>
+    <t>pev_sales_scaler</t>
+  </si>
+  <si>
+    <t>thru2060; new learning; 125K bev curve; noPHEV</t>
   </si>
 </sst>
 </file>
@@ -2201,10 +2231,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF58B9CD-C45C-4464-97D6-845ECC18E560}">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2233,7 +2263,9 @@
       <c r="A3" t="s">
         <v>277</v>
       </c>
-      <c r="B3" s="1"/>
+      <c r="B3" s="1" t="s">
+        <v>359</v>
+      </c>
     </row>
     <row r="4" spans="1:4" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
@@ -2256,7 +2288,7 @@
         <v>211</v>
       </c>
       <c r="B6" s="1">
-        <v>2050</v>
+        <v>2060</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -2349,6 +2381,78 @@
       </c>
       <c r="B16" s="1">
         <v>1.2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>350</v>
+      </c>
+      <c r="B17" s="1">
+        <v>-0.245</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>352</v>
+      </c>
+      <c r="B18" s="1">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>354</v>
+      </c>
+      <c r="B19" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>353</v>
+      </c>
+      <c r="B20" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>355</v>
+      </c>
+      <c r="B21" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>351</v>
+      </c>
+      <c r="B22" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>356</v>
+      </c>
+      <c r="B23" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>357</v>
+      </c>
+      <c r="B24" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>358</v>
+      </c>
+      <c r="B25" s="1">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -7693,7 +7797,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2A32868-5770-4D9F-98C2-1E495D488F86}">
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:E17"/>
     </sheetView>
   </sheetViews>
@@ -10261,7 +10365,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D89349C-4881-488D-B8C5-0F08759EC631}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -10297,16 +10403,16 @@
         <v>275</v>
       </c>
       <c r="B2" s="1">
-        <v>-9.556E-5</v>
+        <v>-1.0551E-4</v>
       </c>
       <c r="C2" s="1">
-        <v>2.652171E-2</v>
+        <v>2.9542829999999999E-2</v>
       </c>
       <c r="D2" s="1">
-        <v>-2.5608517599999998</v>
+        <v>-2.8940968100000002</v>
       </c>
       <c r="E2" s="1">
-        <v>193.19055123999999</v>
+        <v>218.42199600000001</v>
       </c>
       <c r="F2" s="1">
         <v>2019</v>

</xml_diff>

<commit_message>
Update to latest version.
</commit_message>
<xml_diff>
--- a/omega_preproc/alpha_package_costs/inputs/alpha_package_costs_module_inputs.xlsx
+++ b/omega_preproc/alpha_package_costs/inputs/alpha_package_costs_module_inputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TSHERWOO\PycharmProjects\EPA_OMEGA_Model\omega_preproc\alpha_package_costs\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0AAB228-2CD3-48F9-8C6E-FF5CDF2B7A1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBD1E6E4-F028-4BD9-AC40-D6E25D1F364F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="826" xr2:uid="{31AE0ECC-ADD6-46A3-9F50-4BA6582DDF8B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="826" xr2:uid="{31AE0ECC-ADD6-46A3-9F50-4BA6582DDF8B}"/>
   </bookViews>
   <sheets>
     <sheet name="inputs_code" sheetId="15" r:id="rId1"/>
@@ -2234,7 +2234,7 @@
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>